<commit_message>
added results 4d and 4e
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sofia/Desktop/cognitive-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fairouz\Desktop\cognitive project\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0915572-A697-B848-BA65-4CCE25C44799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0FA808-9912-46FA-9F24-04856CCB2281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="500" windowWidth="27140" windowHeight="16440" xr2:uid="{EFD26FD0-07EC-0644-AECA-4418AC46A54A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{EFD26FD0-07EC-0644-AECA-4418AC46A54A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
@@ -459,7 +459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -505,6 +505,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,912 +825,912 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A8C6A9-729D-1346-9EE7-9CB9A898ACBA}">
   <dimension ref="A1:Q99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q26" sqref="Q26"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="56.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="56.6484375" customWidth="1"/>
+    <col min="2" max="2" width="14.1484375" customWidth="1"/>
+    <col min="3" max="3" width="13.1484375" customWidth="1"/>
+    <col min="4" max="4" width="12.84765625" customWidth="1"/>
+    <col min="5" max="5" width="13.6484375" customWidth="1"/>
     <col min="6" max="7" width="13" customWidth="1"/>
-    <col min="8" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="8" max="9" width="12.6484375" customWidth="1"/>
+    <col min="10" max="10" width="11.34765625" customWidth="1"/>
+    <col min="11" max="11" width="12.34765625" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" customWidth="1"/>
-    <col min="14" max="14" width="12.1640625" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" customWidth="1"/>
-    <col min="16" max="17" width="12.33203125" customWidth="1"/>
-    <col min="259" max="259" width="56.6640625" customWidth="1"/>
-    <col min="260" max="260" width="14.1640625" customWidth="1"/>
-    <col min="261" max="261" width="13.1640625" customWidth="1"/>
-    <col min="262" max="262" width="12.83203125" customWidth="1"/>
-    <col min="263" max="263" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.84765625" customWidth="1"/>
+    <col min="14" max="14" width="12.1484375" customWidth="1"/>
+    <col min="15" max="15" width="11.6484375" customWidth="1"/>
+    <col min="16" max="17" width="12.34765625" customWidth="1"/>
+    <col min="259" max="259" width="56.6484375" customWidth="1"/>
+    <col min="260" max="260" width="14.1484375" customWidth="1"/>
+    <col min="261" max="261" width="13.1484375" customWidth="1"/>
+    <col min="262" max="262" width="12.84765625" customWidth="1"/>
+    <col min="263" max="263" width="13.6484375" customWidth="1"/>
     <col min="264" max="265" width="13" customWidth="1"/>
-    <col min="266" max="266" width="12.6640625" customWidth="1"/>
-    <col min="267" max="267" width="11.33203125" customWidth="1"/>
-    <col min="268" max="268" width="12.33203125" customWidth="1"/>
+    <col min="266" max="266" width="12.6484375" customWidth="1"/>
+    <col min="267" max="267" width="11.34765625" customWidth="1"/>
+    <col min="268" max="268" width="12.34765625" customWidth="1"/>
     <col min="269" max="269" width="13" customWidth="1"/>
-    <col min="270" max="270" width="11.83203125" customWidth="1"/>
-    <col min="271" max="271" width="12.1640625" customWidth="1"/>
-    <col min="272" max="272" width="11.6640625" customWidth="1"/>
-    <col min="273" max="273" width="12.33203125" customWidth="1"/>
-    <col min="515" max="515" width="56.6640625" customWidth="1"/>
-    <col min="516" max="516" width="14.1640625" customWidth="1"/>
-    <col min="517" max="517" width="13.1640625" customWidth="1"/>
-    <col min="518" max="518" width="12.83203125" customWidth="1"/>
-    <col min="519" max="519" width="13.6640625" customWidth="1"/>
+    <col min="270" max="270" width="11.84765625" customWidth="1"/>
+    <col min="271" max="271" width="12.1484375" customWidth="1"/>
+    <col min="272" max="272" width="11.6484375" customWidth="1"/>
+    <col min="273" max="273" width="12.34765625" customWidth="1"/>
+    <col min="515" max="515" width="56.6484375" customWidth="1"/>
+    <col min="516" max="516" width="14.1484375" customWidth="1"/>
+    <col min="517" max="517" width="13.1484375" customWidth="1"/>
+    <col min="518" max="518" width="12.84765625" customWidth="1"/>
+    <col min="519" max="519" width="13.6484375" customWidth="1"/>
     <col min="520" max="521" width="13" customWidth="1"/>
-    <col min="522" max="522" width="12.6640625" customWidth="1"/>
-    <col min="523" max="523" width="11.33203125" customWidth="1"/>
-    <col min="524" max="524" width="12.33203125" customWidth="1"/>
+    <col min="522" max="522" width="12.6484375" customWidth="1"/>
+    <col min="523" max="523" width="11.34765625" customWidth="1"/>
+    <col min="524" max="524" width="12.34765625" customWidth="1"/>
     <col min="525" max="525" width="13" customWidth="1"/>
-    <col min="526" max="526" width="11.83203125" customWidth="1"/>
-    <col min="527" max="527" width="12.1640625" customWidth="1"/>
-    <col min="528" max="528" width="11.6640625" customWidth="1"/>
-    <col min="529" max="529" width="12.33203125" customWidth="1"/>
-    <col min="771" max="771" width="56.6640625" customWidth="1"/>
-    <col min="772" max="772" width="14.1640625" customWidth="1"/>
-    <col min="773" max="773" width="13.1640625" customWidth="1"/>
-    <col min="774" max="774" width="12.83203125" customWidth="1"/>
-    <col min="775" max="775" width="13.6640625" customWidth="1"/>
+    <col min="526" max="526" width="11.84765625" customWidth="1"/>
+    <col min="527" max="527" width="12.1484375" customWidth="1"/>
+    <col min="528" max="528" width="11.6484375" customWidth="1"/>
+    <col min="529" max="529" width="12.34765625" customWidth="1"/>
+    <col min="771" max="771" width="56.6484375" customWidth="1"/>
+    <col min="772" max="772" width="14.1484375" customWidth="1"/>
+    <col min="773" max="773" width="13.1484375" customWidth="1"/>
+    <col min="774" max="774" width="12.84765625" customWidth="1"/>
+    <col min="775" max="775" width="13.6484375" customWidth="1"/>
     <col min="776" max="777" width="13" customWidth="1"/>
-    <col min="778" max="778" width="12.6640625" customWidth="1"/>
-    <col min="779" max="779" width="11.33203125" customWidth="1"/>
-    <col min="780" max="780" width="12.33203125" customWidth="1"/>
+    <col min="778" max="778" width="12.6484375" customWidth="1"/>
+    <col min="779" max="779" width="11.34765625" customWidth="1"/>
+    <col min="780" max="780" width="12.34765625" customWidth="1"/>
     <col min="781" max="781" width="13" customWidth="1"/>
-    <col min="782" max="782" width="11.83203125" customWidth="1"/>
-    <col min="783" max="783" width="12.1640625" customWidth="1"/>
-    <col min="784" max="784" width="11.6640625" customWidth="1"/>
-    <col min="785" max="785" width="12.33203125" customWidth="1"/>
-    <col min="1027" max="1027" width="56.6640625" customWidth="1"/>
-    <col min="1028" max="1028" width="14.1640625" customWidth="1"/>
-    <col min="1029" max="1029" width="13.1640625" customWidth="1"/>
-    <col min="1030" max="1030" width="12.83203125" customWidth="1"/>
-    <col min="1031" max="1031" width="13.6640625" customWidth="1"/>
+    <col min="782" max="782" width="11.84765625" customWidth="1"/>
+    <col min="783" max="783" width="12.1484375" customWidth="1"/>
+    <col min="784" max="784" width="11.6484375" customWidth="1"/>
+    <col min="785" max="785" width="12.34765625" customWidth="1"/>
+    <col min="1027" max="1027" width="56.6484375" customWidth="1"/>
+    <col min="1028" max="1028" width="14.1484375" customWidth="1"/>
+    <col min="1029" max="1029" width="13.1484375" customWidth="1"/>
+    <col min="1030" max="1030" width="12.84765625" customWidth="1"/>
+    <col min="1031" max="1031" width="13.6484375" customWidth="1"/>
     <col min="1032" max="1033" width="13" customWidth="1"/>
-    <col min="1034" max="1034" width="12.6640625" customWidth="1"/>
-    <col min="1035" max="1035" width="11.33203125" customWidth="1"/>
-    <col min="1036" max="1036" width="12.33203125" customWidth="1"/>
+    <col min="1034" max="1034" width="12.6484375" customWidth="1"/>
+    <col min="1035" max="1035" width="11.34765625" customWidth="1"/>
+    <col min="1036" max="1036" width="12.34765625" customWidth="1"/>
     <col min="1037" max="1037" width="13" customWidth="1"/>
-    <col min="1038" max="1038" width="11.83203125" customWidth="1"/>
-    <col min="1039" max="1039" width="12.1640625" customWidth="1"/>
-    <col min="1040" max="1040" width="11.6640625" customWidth="1"/>
-    <col min="1041" max="1041" width="12.33203125" customWidth="1"/>
-    <col min="1283" max="1283" width="56.6640625" customWidth="1"/>
-    <col min="1284" max="1284" width="14.1640625" customWidth="1"/>
-    <col min="1285" max="1285" width="13.1640625" customWidth="1"/>
-    <col min="1286" max="1286" width="12.83203125" customWidth="1"/>
-    <col min="1287" max="1287" width="13.6640625" customWidth="1"/>
+    <col min="1038" max="1038" width="11.84765625" customWidth="1"/>
+    <col min="1039" max="1039" width="12.1484375" customWidth="1"/>
+    <col min="1040" max="1040" width="11.6484375" customWidth="1"/>
+    <col min="1041" max="1041" width="12.34765625" customWidth="1"/>
+    <col min="1283" max="1283" width="56.6484375" customWidth="1"/>
+    <col min="1284" max="1284" width="14.1484375" customWidth="1"/>
+    <col min="1285" max="1285" width="13.1484375" customWidth="1"/>
+    <col min="1286" max="1286" width="12.84765625" customWidth="1"/>
+    <col min="1287" max="1287" width="13.6484375" customWidth="1"/>
     <col min="1288" max="1289" width="13" customWidth="1"/>
-    <col min="1290" max="1290" width="12.6640625" customWidth="1"/>
-    <col min="1291" max="1291" width="11.33203125" customWidth="1"/>
-    <col min="1292" max="1292" width="12.33203125" customWidth="1"/>
+    <col min="1290" max="1290" width="12.6484375" customWidth="1"/>
+    <col min="1291" max="1291" width="11.34765625" customWidth="1"/>
+    <col min="1292" max="1292" width="12.34765625" customWidth="1"/>
     <col min="1293" max="1293" width="13" customWidth="1"/>
-    <col min="1294" max="1294" width="11.83203125" customWidth="1"/>
-    <col min="1295" max="1295" width="12.1640625" customWidth="1"/>
-    <col min="1296" max="1296" width="11.6640625" customWidth="1"/>
-    <col min="1297" max="1297" width="12.33203125" customWidth="1"/>
-    <col min="1539" max="1539" width="56.6640625" customWidth="1"/>
-    <col min="1540" max="1540" width="14.1640625" customWidth="1"/>
-    <col min="1541" max="1541" width="13.1640625" customWidth="1"/>
-    <col min="1542" max="1542" width="12.83203125" customWidth="1"/>
-    <col min="1543" max="1543" width="13.6640625" customWidth="1"/>
+    <col min="1294" max="1294" width="11.84765625" customWidth="1"/>
+    <col min="1295" max="1295" width="12.1484375" customWidth="1"/>
+    <col min="1296" max="1296" width="11.6484375" customWidth="1"/>
+    <col min="1297" max="1297" width="12.34765625" customWidth="1"/>
+    <col min="1539" max="1539" width="56.6484375" customWidth="1"/>
+    <col min="1540" max="1540" width="14.1484375" customWidth="1"/>
+    <col min="1541" max="1541" width="13.1484375" customWidth="1"/>
+    <col min="1542" max="1542" width="12.84765625" customWidth="1"/>
+    <col min="1543" max="1543" width="13.6484375" customWidth="1"/>
     <col min="1544" max="1545" width="13" customWidth="1"/>
-    <col min="1546" max="1546" width="12.6640625" customWidth="1"/>
-    <col min="1547" max="1547" width="11.33203125" customWidth="1"/>
-    <col min="1548" max="1548" width="12.33203125" customWidth="1"/>
+    <col min="1546" max="1546" width="12.6484375" customWidth="1"/>
+    <col min="1547" max="1547" width="11.34765625" customWidth="1"/>
+    <col min="1548" max="1548" width="12.34765625" customWidth="1"/>
     <col min="1549" max="1549" width="13" customWidth="1"/>
-    <col min="1550" max="1550" width="11.83203125" customWidth="1"/>
-    <col min="1551" max="1551" width="12.1640625" customWidth="1"/>
-    <col min="1552" max="1552" width="11.6640625" customWidth="1"/>
-    <col min="1553" max="1553" width="12.33203125" customWidth="1"/>
-    <col min="1795" max="1795" width="56.6640625" customWidth="1"/>
-    <col min="1796" max="1796" width="14.1640625" customWidth="1"/>
-    <col min="1797" max="1797" width="13.1640625" customWidth="1"/>
-    <col min="1798" max="1798" width="12.83203125" customWidth="1"/>
-    <col min="1799" max="1799" width="13.6640625" customWidth="1"/>
+    <col min="1550" max="1550" width="11.84765625" customWidth="1"/>
+    <col min="1551" max="1551" width="12.1484375" customWidth="1"/>
+    <col min="1552" max="1552" width="11.6484375" customWidth="1"/>
+    <col min="1553" max="1553" width="12.34765625" customWidth="1"/>
+    <col min="1795" max="1795" width="56.6484375" customWidth="1"/>
+    <col min="1796" max="1796" width="14.1484375" customWidth="1"/>
+    <col min="1797" max="1797" width="13.1484375" customWidth="1"/>
+    <col min="1798" max="1798" width="12.84765625" customWidth="1"/>
+    <col min="1799" max="1799" width="13.6484375" customWidth="1"/>
     <col min="1800" max="1801" width="13" customWidth="1"/>
-    <col min="1802" max="1802" width="12.6640625" customWidth="1"/>
-    <col min="1803" max="1803" width="11.33203125" customWidth="1"/>
-    <col min="1804" max="1804" width="12.33203125" customWidth="1"/>
+    <col min="1802" max="1802" width="12.6484375" customWidth="1"/>
+    <col min="1803" max="1803" width="11.34765625" customWidth="1"/>
+    <col min="1804" max="1804" width="12.34765625" customWidth="1"/>
     <col min="1805" max="1805" width="13" customWidth="1"/>
-    <col min="1806" max="1806" width="11.83203125" customWidth="1"/>
-    <col min="1807" max="1807" width="12.1640625" customWidth="1"/>
-    <col min="1808" max="1808" width="11.6640625" customWidth="1"/>
-    <col min="1809" max="1809" width="12.33203125" customWidth="1"/>
-    <col min="2051" max="2051" width="56.6640625" customWidth="1"/>
-    <col min="2052" max="2052" width="14.1640625" customWidth="1"/>
-    <col min="2053" max="2053" width="13.1640625" customWidth="1"/>
-    <col min="2054" max="2054" width="12.83203125" customWidth="1"/>
-    <col min="2055" max="2055" width="13.6640625" customWidth="1"/>
+    <col min="1806" max="1806" width="11.84765625" customWidth="1"/>
+    <col min="1807" max="1807" width="12.1484375" customWidth="1"/>
+    <col min="1808" max="1808" width="11.6484375" customWidth="1"/>
+    <col min="1809" max="1809" width="12.34765625" customWidth="1"/>
+    <col min="2051" max="2051" width="56.6484375" customWidth="1"/>
+    <col min="2052" max="2052" width="14.1484375" customWidth="1"/>
+    <col min="2053" max="2053" width="13.1484375" customWidth="1"/>
+    <col min="2054" max="2054" width="12.84765625" customWidth="1"/>
+    <col min="2055" max="2055" width="13.6484375" customWidth="1"/>
     <col min="2056" max="2057" width="13" customWidth="1"/>
-    <col min="2058" max="2058" width="12.6640625" customWidth="1"/>
-    <col min="2059" max="2059" width="11.33203125" customWidth="1"/>
-    <col min="2060" max="2060" width="12.33203125" customWidth="1"/>
+    <col min="2058" max="2058" width="12.6484375" customWidth="1"/>
+    <col min="2059" max="2059" width="11.34765625" customWidth="1"/>
+    <col min="2060" max="2060" width="12.34765625" customWidth="1"/>
     <col min="2061" max="2061" width="13" customWidth="1"/>
-    <col min="2062" max="2062" width="11.83203125" customWidth="1"/>
-    <col min="2063" max="2063" width="12.1640625" customWidth="1"/>
-    <col min="2064" max="2064" width="11.6640625" customWidth="1"/>
-    <col min="2065" max="2065" width="12.33203125" customWidth="1"/>
-    <col min="2307" max="2307" width="56.6640625" customWidth="1"/>
-    <col min="2308" max="2308" width="14.1640625" customWidth="1"/>
-    <col min="2309" max="2309" width="13.1640625" customWidth="1"/>
-    <col min="2310" max="2310" width="12.83203125" customWidth="1"/>
-    <col min="2311" max="2311" width="13.6640625" customWidth="1"/>
+    <col min="2062" max="2062" width="11.84765625" customWidth="1"/>
+    <col min="2063" max="2063" width="12.1484375" customWidth="1"/>
+    <col min="2064" max="2064" width="11.6484375" customWidth="1"/>
+    <col min="2065" max="2065" width="12.34765625" customWidth="1"/>
+    <col min="2307" max="2307" width="56.6484375" customWidth="1"/>
+    <col min="2308" max="2308" width="14.1484375" customWidth="1"/>
+    <col min="2309" max="2309" width="13.1484375" customWidth="1"/>
+    <col min="2310" max="2310" width="12.84765625" customWidth="1"/>
+    <col min="2311" max="2311" width="13.6484375" customWidth="1"/>
     <col min="2312" max="2313" width="13" customWidth="1"/>
-    <col min="2314" max="2314" width="12.6640625" customWidth="1"/>
-    <col min="2315" max="2315" width="11.33203125" customWidth="1"/>
-    <col min="2316" max="2316" width="12.33203125" customWidth="1"/>
+    <col min="2314" max="2314" width="12.6484375" customWidth="1"/>
+    <col min="2315" max="2315" width="11.34765625" customWidth="1"/>
+    <col min="2316" max="2316" width="12.34765625" customWidth="1"/>
     <col min="2317" max="2317" width="13" customWidth="1"/>
-    <col min="2318" max="2318" width="11.83203125" customWidth="1"/>
-    <col min="2319" max="2319" width="12.1640625" customWidth="1"/>
-    <col min="2320" max="2320" width="11.6640625" customWidth="1"/>
-    <col min="2321" max="2321" width="12.33203125" customWidth="1"/>
-    <col min="2563" max="2563" width="56.6640625" customWidth="1"/>
-    <col min="2564" max="2564" width="14.1640625" customWidth="1"/>
-    <col min="2565" max="2565" width="13.1640625" customWidth="1"/>
-    <col min="2566" max="2566" width="12.83203125" customWidth="1"/>
-    <col min="2567" max="2567" width="13.6640625" customWidth="1"/>
+    <col min="2318" max="2318" width="11.84765625" customWidth="1"/>
+    <col min="2319" max="2319" width="12.1484375" customWidth="1"/>
+    <col min="2320" max="2320" width="11.6484375" customWidth="1"/>
+    <col min="2321" max="2321" width="12.34765625" customWidth="1"/>
+    <col min="2563" max="2563" width="56.6484375" customWidth="1"/>
+    <col min="2564" max="2564" width="14.1484375" customWidth="1"/>
+    <col min="2565" max="2565" width="13.1484375" customWidth="1"/>
+    <col min="2566" max="2566" width="12.84765625" customWidth="1"/>
+    <col min="2567" max="2567" width="13.6484375" customWidth="1"/>
     <col min="2568" max="2569" width="13" customWidth="1"/>
-    <col min="2570" max="2570" width="12.6640625" customWidth="1"/>
-    <col min="2571" max="2571" width="11.33203125" customWidth="1"/>
-    <col min="2572" max="2572" width="12.33203125" customWidth="1"/>
+    <col min="2570" max="2570" width="12.6484375" customWidth="1"/>
+    <col min="2571" max="2571" width="11.34765625" customWidth="1"/>
+    <col min="2572" max="2572" width="12.34765625" customWidth="1"/>
     <col min="2573" max="2573" width="13" customWidth="1"/>
-    <col min="2574" max="2574" width="11.83203125" customWidth="1"/>
-    <col min="2575" max="2575" width="12.1640625" customWidth="1"/>
-    <col min="2576" max="2576" width="11.6640625" customWidth="1"/>
-    <col min="2577" max="2577" width="12.33203125" customWidth="1"/>
-    <col min="2819" max="2819" width="56.6640625" customWidth="1"/>
-    <col min="2820" max="2820" width="14.1640625" customWidth="1"/>
-    <col min="2821" max="2821" width="13.1640625" customWidth="1"/>
-    <col min="2822" max="2822" width="12.83203125" customWidth="1"/>
-    <col min="2823" max="2823" width="13.6640625" customWidth="1"/>
+    <col min="2574" max="2574" width="11.84765625" customWidth="1"/>
+    <col min="2575" max="2575" width="12.1484375" customWidth="1"/>
+    <col min="2576" max="2576" width="11.6484375" customWidth="1"/>
+    <col min="2577" max="2577" width="12.34765625" customWidth="1"/>
+    <col min="2819" max="2819" width="56.6484375" customWidth="1"/>
+    <col min="2820" max="2820" width="14.1484375" customWidth="1"/>
+    <col min="2821" max="2821" width="13.1484375" customWidth="1"/>
+    <col min="2822" max="2822" width="12.84765625" customWidth="1"/>
+    <col min="2823" max="2823" width="13.6484375" customWidth="1"/>
     <col min="2824" max="2825" width="13" customWidth="1"/>
-    <col min="2826" max="2826" width="12.6640625" customWidth="1"/>
-    <col min="2827" max="2827" width="11.33203125" customWidth="1"/>
-    <col min="2828" max="2828" width="12.33203125" customWidth="1"/>
+    <col min="2826" max="2826" width="12.6484375" customWidth="1"/>
+    <col min="2827" max="2827" width="11.34765625" customWidth="1"/>
+    <col min="2828" max="2828" width="12.34765625" customWidth="1"/>
     <col min="2829" max="2829" width="13" customWidth="1"/>
-    <col min="2830" max="2830" width="11.83203125" customWidth="1"/>
-    <col min="2831" max="2831" width="12.1640625" customWidth="1"/>
-    <col min="2832" max="2832" width="11.6640625" customWidth="1"/>
-    <col min="2833" max="2833" width="12.33203125" customWidth="1"/>
-    <col min="3075" max="3075" width="56.6640625" customWidth="1"/>
-    <col min="3076" max="3076" width="14.1640625" customWidth="1"/>
-    <col min="3077" max="3077" width="13.1640625" customWidth="1"/>
-    <col min="3078" max="3078" width="12.83203125" customWidth="1"/>
-    <col min="3079" max="3079" width="13.6640625" customWidth="1"/>
+    <col min="2830" max="2830" width="11.84765625" customWidth="1"/>
+    <col min="2831" max="2831" width="12.1484375" customWidth="1"/>
+    <col min="2832" max="2832" width="11.6484375" customWidth="1"/>
+    <col min="2833" max="2833" width="12.34765625" customWidth="1"/>
+    <col min="3075" max="3075" width="56.6484375" customWidth="1"/>
+    <col min="3076" max="3076" width="14.1484375" customWidth="1"/>
+    <col min="3077" max="3077" width="13.1484375" customWidth="1"/>
+    <col min="3078" max="3078" width="12.84765625" customWidth="1"/>
+    <col min="3079" max="3079" width="13.6484375" customWidth="1"/>
     <col min="3080" max="3081" width="13" customWidth="1"/>
-    <col min="3082" max="3082" width="12.6640625" customWidth="1"/>
-    <col min="3083" max="3083" width="11.33203125" customWidth="1"/>
-    <col min="3084" max="3084" width="12.33203125" customWidth="1"/>
+    <col min="3082" max="3082" width="12.6484375" customWidth="1"/>
+    <col min="3083" max="3083" width="11.34765625" customWidth="1"/>
+    <col min="3084" max="3084" width="12.34765625" customWidth="1"/>
     <col min="3085" max="3085" width="13" customWidth="1"/>
-    <col min="3086" max="3086" width="11.83203125" customWidth="1"/>
-    <col min="3087" max="3087" width="12.1640625" customWidth="1"/>
-    <col min="3088" max="3088" width="11.6640625" customWidth="1"/>
-    <col min="3089" max="3089" width="12.33203125" customWidth="1"/>
-    <col min="3331" max="3331" width="56.6640625" customWidth="1"/>
-    <col min="3332" max="3332" width="14.1640625" customWidth="1"/>
-    <col min="3333" max="3333" width="13.1640625" customWidth="1"/>
-    <col min="3334" max="3334" width="12.83203125" customWidth="1"/>
-    <col min="3335" max="3335" width="13.6640625" customWidth="1"/>
+    <col min="3086" max="3086" width="11.84765625" customWidth="1"/>
+    <col min="3087" max="3087" width="12.1484375" customWidth="1"/>
+    <col min="3088" max="3088" width="11.6484375" customWidth="1"/>
+    <col min="3089" max="3089" width="12.34765625" customWidth="1"/>
+    <col min="3331" max="3331" width="56.6484375" customWidth="1"/>
+    <col min="3332" max="3332" width="14.1484375" customWidth="1"/>
+    <col min="3333" max="3333" width="13.1484375" customWidth="1"/>
+    <col min="3334" max="3334" width="12.84765625" customWidth="1"/>
+    <col min="3335" max="3335" width="13.6484375" customWidth="1"/>
     <col min="3336" max="3337" width="13" customWidth="1"/>
-    <col min="3338" max="3338" width="12.6640625" customWidth="1"/>
-    <col min="3339" max="3339" width="11.33203125" customWidth="1"/>
-    <col min="3340" max="3340" width="12.33203125" customWidth="1"/>
+    <col min="3338" max="3338" width="12.6484375" customWidth="1"/>
+    <col min="3339" max="3339" width="11.34765625" customWidth="1"/>
+    <col min="3340" max="3340" width="12.34765625" customWidth="1"/>
     <col min="3341" max="3341" width="13" customWidth="1"/>
-    <col min="3342" max="3342" width="11.83203125" customWidth="1"/>
-    <col min="3343" max="3343" width="12.1640625" customWidth="1"/>
-    <col min="3344" max="3344" width="11.6640625" customWidth="1"/>
-    <col min="3345" max="3345" width="12.33203125" customWidth="1"/>
-    <col min="3587" max="3587" width="56.6640625" customWidth="1"/>
-    <col min="3588" max="3588" width="14.1640625" customWidth="1"/>
-    <col min="3589" max="3589" width="13.1640625" customWidth="1"/>
-    <col min="3590" max="3590" width="12.83203125" customWidth="1"/>
-    <col min="3591" max="3591" width="13.6640625" customWidth="1"/>
+    <col min="3342" max="3342" width="11.84765625" customWidth="1"/>
+    <col min="3343" max="3343" width="12.1484375" customWidth="1"/>
+    <col min="3344" max="3344" width="11.6484375" customWidth="1"/>
+    <col min="3345" max="3345" width="12.34765625" customWidth="1"/>
+    <col min="3587" max="3587" width="56.6484375" customWidth="1"/>
+    <col min="3588" max="3588" width="14.1484375" customWidth="1"/>
+    <col min="3589" max="3589" width="13.1484375" customWidth="1"/>
+    <col min="3590" max="3590" width="12.84765625" customWidth="1"/>
+    <col min="3591" max="3591" width="13.6484375" customWidth="1"/>
     <col min="3592" max="3593" width="13" customWidth="1"/>
-    <col min="3594" max="3594" width="12.6640625" customWidth="1"/>
-    <col min="3595" max="3595" width="11.33203125" customWidth="1"/>
-    <col min="3596" max="3596" width="12.33203125" customWidth="1"/>
+    <col min="3594" max="3594" width="12.6484375" customWidth="1"/>
+    <col min="3595" max="3595" width="11.34765625" customWidth="1"/>
+    <col min="3596" max="3596" width="12.34765625" customWidth="1"/>
     <col min="3597" max="3597" width="13" customWidth="1"/>
-    <col min="3598" max="3598" width="11.83203125" customWidth="1"/>
-    <col min="3599" max="3599" width="12.1640625" customWidth="1"/>
-    <col min="3600" max="3600" width="11.6640625" customWidth="1"/>
-    <col min="3601" max="3601" width="12.33203125" customWidth="1"/>
-    <col min="3843" max="3843" width="56.6640625" customWidth="1"/>
-    <col min="3844" max="3844" width="14.1640625" customWidth="1"/>
-    <col min="3845" max="3845" width="13.1640625" customWidth="1"/>
-    <col min="3846" max="3846" width="12.83203125" customWidth="1"/>
-    <col min="3847" max="3847" width="13.6640625" customWidth="1"/>
+    <col min="3598" max="3598" width="11.84765625" customWidth="1"/>
+    <col min="3599" max="3599" width="12.1484375" customWidth="1"/>
+    <col min="3600" max="3600" width="11.6484375" customWidth="1"/>
+    <col min="3601" max="3601" width="12.34765625" customWidth="1"/>
+    <col min="3843" max="3843" width="56.6484375" customWidth="1"/>
+    <col min="3844" max="3844" width="14.1484375" customWidth="1"/>
+    <col min="3845" max="3845" width="13.1484375" customWidth="1"/>
+    <col min="3846" max="3846" width="12.84765625" customWidth="1"/>
+    <col min="3847" max="3847" width="13.6484375" customWidth="1"/>
     <col min="3848" max="3849" width="13" customWidth="1"/>
-    <col min="3850" max="3850" width="12.6640625" customWidth="1"/>
-    <col min="3851" max="3851" width="11.33203125" customWidth="1"/>
-    <col min="3852" max="3852" width="12.33203125" customWidth="1"/>
+    <col min="3850" max="3850" width="12.6484375" customWidth="1"/>
+    <col min="3851" max="3851" width="11.34765625" customWidth="1"/>
+    <col min="3852" max="3852" width="12.34765625" customWidth="1"/>
     <col min="3853" max="3853" width="13" customWidth="1"/>
-    <col min="3854" max="3854" width="11.83203125" customWidth="1"/>
-    <col min="3855" max="3855" width="12.1640625" customWidth="1"/>
-    <col min="3856" max="3856" width="11.6640625" customWidth="1"/>
-    <col min="3857" max="3857" width="12.33203125" customWidth="1"/>
-    <col min="4099" max="4099" width="56.6640625" customWidth="1"/>
-    <col min="4100" max="4100" width="14.1640625" customWidth="1"/>
-    <col min="4101" max="4101" width="13.1640625" customWidth="1"/>
-    <col min="4102" max="4102" width="12.83203125" customWidth="1"/>
-    <col min="4103" max="4103" width="13.6640625" customWidth="1"/>
+    <col min="3854" max="3854" width="11.84765625" customWidth="1"/>
+    <col min="3855" max="3855" width="12.1484375" customWidth="1"/>
+    <col min="3856" max="3856" width="11.6484375" customWidth="1"/>
+    <col min="3857" max="3857" width="12.34765625" customWidth="1"/>
+    <col min="4099" max="4099" width="56.6484375" customWidth="1"/>
+    <col min="4100" max="4100" width="14.1484375" customWidth="1"/>
+    <col min="4101" max="4101" width="13.1484375" customWidth="1"/>
+    <col min="4102" max="4102" width="12.84765625" customWidth="1"/>
+    <col min="4103" max="4103" width="13.6484375" customWidth="1"/>
     <col min="4104" max="4105" width="13" customWidth="1"/>
-    <col min="4106" max="4106" width="12.6640625" customWidth="1"/>
-    <col min="4107" max="4107" width="11.33203125" customWidth="1"/>
-    <col min="4108" max="4108" width="12.33203125" customWidth="1"/>
+    <col min="4106" max="4106" width="12.6484375" customWidth="1"/>
+    <col min="4107" max="4107" width="11.34765625" customWidth="1"/>
+    <col min="4108" max="4108" width="12.34765625" customWidth="1"/>
     <col min="4109" max="4109" width="13" customWidth="1"/>
-    <col min="4110" max="4110" width="11.83203125" customWidth="1"/>
-    <col min="4111" max="4111" width="12.1640625" customWidth="1"/>
-    <col min="4112" max="4112" width="11.6640625" customWidth="1"/>
-    <col min="4113" max="4113" width="12.33203125" customWidth="1"/>
-    <col min="4355" max="4355" width="56.6640625" customWidth="1"/>
-    <col min="4356" max="4356" width="14.1640625" customWidth="1"/>
-    <col min="4357" max="4357" width="13.1640625" customWidth="1"/>
-    <col min="4358" max="4358" width="12.83203125" customWidth="1"/>
-    <col min="4359" max="4359" width="13.6640625" customWidth="1"/>
+    <col min="4110" max="4110" width="11.84765625" customWidth="1"/>
+    <col min="4111" max="4111" width="12.1484375" customWidth="1"/>
+    <col min="4112" max="4112" width="11.6484375" customWidth="1"/>
+    <col min="4113" max="4113" width="12.34765625" customWidth="1"/>
+    <col min="4355" max="4355" width="56.6484375" customWidth="1"/>
+    <col min="4356" max="4356" width="14.1484375" customWidth="1"/>
+    <col min="4357" max="4357" width="13.1484375" customWidth="1"/>
+    <col min="4358" max="4358" width="12.84765625" customWidth="1"/>
+    <col min="4359" max="4359" width="13.6484375" customWidth="1"/>
     <col min="4360" max="4361" width="13" customWidth="1"/>
-    <col min="4362" max="4362" width="12.6640625" customWidth="1"/>
-    <col min="4363" max="4363" width="11.33203125" customWidth="1"/>
-    <col min="4364" max="4364" width="12.33203125" customWidth="1"/>
+    <col min="4362" max="4362" width="12.6484375" customWidth="1"/>
+    <col min="4363" max="4363" width="11.34765625" customWidth="1"/>
+    <col min="4364" max="4364" width="12.34765625" customWidth="1"/>
     <col min="4365" max="4365" width="13" customWidth="1"/>
-    <col min="4366" max="4366" width="11.83203125" customWidth="1"/>
-    <col min="4367" max="4367" width="12.1640625" customWidth="1"/>
-    <col min="4368" max="4368" width="11.6640625" customWidth="1"/>
-    <col min="4369" max="4369" width="12.33203125" customWidth="1"/>
-    <col min="4611" max="4611" width="56.6640625" customWidth="1"/>
-    <col min="4612" max="4612" width="14.1640625" customWidth="1"/>
-    <col min="4613" max="4613" width="13.1640625" customWidth="1"/>
-    <col min="4614" max="4614" width="12.83203125" customWidth="1"/>
-    <col min="4615" max="4615" width="13.6640625" customWidth="1"/>
+    <col min="4366" max="4366" width="11.84765625" customWidth="1"/>
+    <col min="4367" max="4367" width="12.1484375" customWidth="1"/>
+    <col min="4368" max="4368" width="11.6484375" customWidth="1"/>
+    <col min="4369" max="4369" width="12.34765625" customWidth="1"/>
+    <col min="4611" max="4611" width="56.6484375" customWidth="1"/>
+    <col min="4612" max="4612" width="14.1484375" customWidth="1"/>
+    <col min="4613" max="4613" width="13.1484375" customWidth="1"/>
+    <col min="4614" max="4614" width="12.84765625" customWidth="1"/>
+    <col min="4615" max="4615" width="13.6484375" customWidth="1"/>
     <col min="4616" max="4617" width="13" customWidth="1"/>
-    <col min="4618" max="4618" width="12.6640625" customWidth="1"/>
-    <col min="4619" max="4619" width="11.33203125" customWidth="1"/>
-    <col min="4620" max="4620" width="12.33203125" customWidth="1"/>
+    <col min="4618" max="4618" width="12.6484375" customWidth="1"/>
+    <col min="4619" max="4619" width="11.34765625" customWidth="1"/>
+    <col min="4620" max="4620" width="12.34765625" customWidth="1"/>
     <col min="4621" max="4621" width="13" customWidth="1"/>
-    <col min="4622" max="4622" width="11.83203125" customWidth="1"/>
-    <col min="4623" max="4623" width="12.1640625" customWidth="1"/>
-    <col min="4624" max="4624" width="11.6640625" customWidth="1"/>
-    <col min="4625" max="4625" width="12.33203125" customWidth="1"/>
-    <col min="4867" max="4867" width="56.6640625" customWidth="1"/>
-    <col min="4868" max="4868" width="14.1640625" customWidth="1"/>
-    <col min="4869" max="4869" width="13.1640625" customWidth="1"/>
-    <col min="4870" max="4870" width="12.83203125" customWidth="1"/>
-    <col min="4871" max="4871" width="13.6640625" customWidth="1"/>
+    <col min="4622" max="4622" width="11.84765625" customWidth="1"/>
+    <col min="4623" max="4623" width="12.1484375" customWidth="1"/>
+    <col min="4624" max="4624" width="11.6484375" customWidth="1"/>
+    <col min="4625" max="4625" width="12.34765625" customWidth="1"/>
+    <col min="4867" max="4867" width="56.6484375" customWidth="1"/>
+    <col min="4868" max="4868" width="14.1484375" customWidth="1"/>
+    <col min="4869" max="4869" width="13.1484375" customWidth="1"/>
+    <col min="4870" max="4870" width="12.84765625" customWidth="1"/>
+    <col min="4871" max="4871" width="13.6484375" customWidth="1"/>
     <col min="4872" max="4873" width="13" customWidth="1"/>
-    <col min="4874" max="4874" width="12.6640625" customWidth="1"/>
-    <col min="4875" max="4875" width="11.33203125" customWidth="1"/>
-    <col min="4876" max="4876" width="12.33203125" customWidth="1"/>
+    <col min="4874" max="4874" width="12.6484375" customWidth="1"/>
+    <col min="4875" max="4875" width="11.34765625" customWidth="1"/>
+    <col min="4876" max="4876" width="12.34765625" customWidth="1"/>
     <col min="4877" max="4877" width="13" customWidth="1"/>
-    <col min="4878" max="4878" width="11.83203125" customWidth="1"/>
-    <col min="4879" max="4879" width="12.1640625" customWidth="1"/>
-    <col min="4880" max="4880" width="11.6640625" customWidth="1"/>
-    <col min="4881" max="4881" width="12.33203125" customWidth="1"/>
-    <col min="5123" max="5123" width="56.6640625" customWidth="1"/>
-    <col min="5124" max="5124" width="14.1640625" customWidth="1"/>
-    <col min="5125" max="5125" width="13.1640625" customWidth="1"/>
-    <col min="5126" max="5126" width="12.83203125" customWidth="1"/>
-    <col min="5127" max="5127" width="13.6640625" customWidth="1"/>
+    <col min="4878" max="4878" width="11.84765625" customWidth="1"/>
+    <col min="4879" max="4879" width="12.1484375" customWidth="1"/>
+    <col min="4880" max="4880" width="11.6484375" customWidth="1"/>
+    <col min="4881" max="4881" width="12.34765625" customWidth="1"/>
+    <col min="5123" max="5123" width="56.6484375" customWidth="1"/>
+    <col min="5124" max="5124" width="14.1484375" customWidth="1"/>
+    <col min="5125" max="5125" width="13.1484375" customWidth="1"/>
+    <col min="5126" max="5126" width="12.84765625" customWidth="1"/>
+    <col min="5127" max="5127" width="13.6484375" customWidth="1"/>
     <col min="5128" max="5129" width="13" customWidth="1"/>
-    <col min="5130" max="5130" width="12.6640625" customWidth="1"/>
-    <col min="5131" max="5131" width="11.33203125" customWidth="1"/>
-    <col min="5132" max="5132" width="12.33203125" customWidth="1"/>
+    <col min="5130" max="5130" width="12.6484375" customWidth="1"/>
+    <col min="5131" max="5131" width="11.34765625" customWidth="1"/>
+    <col min="5132" max="5132" width="12.34765625" customWidth="1"/>
     <col min="5133" max="5133" width="13" customWidth="1"/>
-    <col min="5134" max="5134" width="11.83203125" customWidth="1"/>
-    <col min="5135" max="5135" width="12.1640625" customWidth="1"/>
-    <col min="5136" max="5136" width="11.6640625" customWidth="1"/>
-    <col min="5137" max="5137" width="12.33203125" customWidth="1"/>
-    <col min="5379" max="5379" width="56.6640625" customWidth="1"/>
-    <col min="5380" max="5380" width="14.1640625" customWidth="1"/>
-    <col min="5381" max="5381" width="13.1640625" customWidth="1"/>
-    <col min="5382" max="5382" width="12.83203125" customWidth="1"/>
-    <col min="5383" max="5383" width="13.6640625" customWidth="1"/>
+    <col min="5134" max="5134" width="11.84765625" customWidth="1"/>
+    <col min="5135" max="5135" width="12.1484375" customWidth="1"/>
+    <col min="5136" max="5136" width="11.6484375" customWidth="1"/>
+    <col min="5137" max="5137" width="12.34765625" customWidth="1"/>
+    <col min="5379" max="5379" width="56.6484375" customWidth="1"/>
+    <col min="5380" max="5380" width="14.1484375" customWidth="1"/>
+    <col min="5381" max="5381" width="13.1484375" customWidth="1"/>
+    <col min="5382" max="5382" width="12.84765625" customWidth="1"/>
+    <col min="5383" max="5383" width="13.6484375" customWidth="1"/>
     <col min="5384" max="5385" width="13" customWidth="1"/>
-    <col min="5386" max="5386" width="12.6640625" customWidth="1"/>
-    <col min="5387" max="5387" width="11.33203125" customWidth="1"/>
-    <col min="5388" max="5388" width="12.33203125" customWidth="1"/>
+    <col min="5386" max="5386" width="12.6484375" customWidth="1"/>
+    <col min="5387" max="5387" width="11.34765625" customWidth="1"/>
+    <col min="5388" max="5388" width="12.34765625" customWidth="1"/>
     <col min="5389" max="5389" width="13" customWidth="1"/>
-    <col min="5390" max="5390" width="11.83203125" customWidth="1"/>
-    <col min="5391" max="5391" width="12.1640625" customWidth="1"/>
-    <col min="5392" max="5392" width="11.6640625" customWidth="1"/>
-    <col min="5393" max="5393" width="12.33203125" customWidth="1"/>
-    <col min="5635" max="5635" width="56.6640625" customWidth="1"/>
-    <col min="5636" max="5636" width="14.1640625" customWidth="1"/>
-    <col min="5637" max="5637" width="13.1640625" customWidth="1"/>
-    <col min="5638" max="5638" width="12.83203125" customWidth="1"/>
-    <col min="5639" max="5639" width="13.6640625" customWidth="1"/>
+    <col min="5390" max="5390" width="11.84765625" customWidth="1"/>
+    <col min="5391" max="5391" width="12.1484375" customWidth="1"/>
+    <col min="5392" max="5392" width="11.6484375" customWidth="1"/>
+    <col min="5393" max="5393" width="12.34765625" customWidth="1"/>
+    <col min="5635" max="5635" width="56.6484375" customWidth="1"/>
+    <col min="5636" max="5636" width="14.1484375" customWidth="1"/>
+    <col min="5637" max="5637" width="13.1484375" customWidth="1"/>
+    <col min="5638" max="5638" width="12.84765625" customWidth="1"/>
+    <col min="5639" max="5639" width="13.6484375" customWidth="1"/>
     <col min="5640" max="5641" width="13" customWidth="1"/>
-    <col min="5642" max="5642" width="12.6640625" customWidth="1"/>
-    <col min="5643" max="5643" width="11.33203125" customWidth="1"/>
-    <col min="5644" max="5644" width="12.33203125" customWidth="1"/>
+    <col min="5642" max="5642" width="12.6484375" customWidth="1"/>
+    <col min="5643" max="5643" width="11.34765625" customWidth="1"/>
+    <col min="5644" max="5644" width="12.34765625" customWidth="1"/>
     <col min="5645" max="5645" width="13" customWidth="1"/>
-    <col min="5646" max="5646" width="11.83203125" customWidth="1"/>
-    <col min="5647" max="5647" width="12.1640625" customWidth="1"/>
-    <col min="5648" max="5648" width="11.6640625" customWidth="1"/>
-    <col min="5649" max="5649" width="12.33203125" customWidth="1"/>
-    <col min="5891" max="5891" width="56.6640625" customWidth="1"/>
-    <col min="5892" max="5892" width="14.1640625" customWidth="1"/>
-    <col min="5893" max="5893" width="13.1640625" customWidth="1"/>
-    <col min="5894" max="5894" width="12.83203125" customWidth="1"/>
-    <col min="5895" max="5895" width="13.6640625" customWidth="1"/>
+    <col min="5646" max="5646" width="11.84765625" customWidth="1"/>
+    <col min="5647" max="5647" width="12.1484375" customWidth="1"/>
+    <col min="5648" max="5648" width="11.6484375" customWidth="1"/>
+    <col min="5649" max="5649" width="12.34765625" customWidth="1"/>
+    <col min="5891" max="5891" width="56.6484375" customWidth="1"/>
+    <col min="5892" max="5892" width="14.1484375" customWidth="1"/>
+    <col min="5893" max="5893" width="13.1484375" customWidth="1"/>
+    <col min="5894" max="5894" width="12.84765625" customWidth="1"/>
+    <col min="5895" max="5895" width="13.6484375" customWidth="1"/>
     <col min="5896" max="5897" width="13" customWidth="1"/>
-    <col min="5898" max="5898" width="12.6640625" customWidth="1"/>
-    <col min="5899" max="5899" width="11.33203125" customWidth="1"/>
-    <col min="5900" max="5900" width="12.33203125" customWidth="1"/>
+    <col min="5898" max="5898" width="12.6484375" customWidth="1"/>
+    <col min="5899" max="5899" width="11.34765625" customWidth="1"/>
+    <col min="5900" max="5900" width="12.34765625" customWidth="1"/>
     <col min="5901" max="5901" width="13" customWidth="1"/>
-    <col min="5902" max="5902" width="11.83203125" customWidth="1"/>
-    <col min="5903" max="5903" width="12.1640625" customWidth="1"/>
-    <col min="5904" max="5904" width="11.6640625" customWidth="1"/>
-    <col min="5905" max="5905" width="12.33203125" customWidth="1"/>
-    <col min="6147" max="6147" width="56.6640625" customWidth="1"/>
-    <col min="6148" max="6148" width="14.1640625" customWidth="1"/>
-    <col min="6149" max="6149" width="13.1640625" customWidth="1"/>
-    <col min="6150" max="6150" width="12.83203125" customWidth="1"/>
-    <col min="6151" max="6151" width="13.6640625" customWidth="1"/>
+    <col min="5902" max="5902" width="11.84765625" customWidth="1"/>
+    <col min="5903" max="5903" width="12.1484375" customWidth="1"/>
+    <col min="5904" max="5904" width="11.6484375" customWidth="1"/>
+    <col min="5905" max="5905" width="12.34765625" customWidth="1"/>
+    <col min="6147" max="6147" width="56.6484375" customWidth="1"/>
+    <col min="6148" max="6148" width="14.1484375" customWidth="1"/>
+    <col min="6149" max="6149" width="13.1484375" customWidth="1"/>
+    <col min="6150" max="6150" width="12.84765625" customWidth="1"/>
+    <col min="6151" max="6151" width="13.6484375" customWidth="1"/>
     <col min="6152" max="6153" width="13" customWidth="1"/>
-    <col min="6154" max="6154" width="12.6640625" customWidth="1"/>
-    <col min="6155" max="6155" width="11.33203125" customWidth="1"/>
-    <col min="6156" max="6156" width="12.33203125" customWidth="1"/>
+    <col min="6154" max="6154" width="12.6484375" customWidth="1"/>
+    <col min="6155" max="6155" width="11.34765625" customWidth="1"/>
+    <col min="6156" max="6156" width="12.34765625" customWidth="1"/>
     <col min="6157" max="6157" width="13" customWidth="1"/>
-    <col min="6158" max="6158" width="11.83203125" customWidth="1"/>
-    <col min="6159" max="6159" width="12.1640625" customWidth="1"/>
-    <col min="6160" max="6160" width="11.6640625" customWidth="1"/>
-    <col min="6161" max="6161" width="12.33203125" customWidth="1"/>
-    <col min="6403" max="6403" width="56.6640625" customWidth="1"/>
-    <col min="6404" max="6404" width="14.1640625" customWidth="1"/>
-    <col min="6405" max="6405" width="13.1640625" customWidth="1"/>
-    <col min="6406" max="6406" width="12.83203125" customWidth="1"/>
-    <col min="6407" max="6407" width="13.6640625" customWidth="1"/>
+    <col min="6158" max="6158" width="11.84765625" customWidth="1"/>
+    <col min="6159" max="6159" width="12.1484375" customWidth="1"/>
+    <col min="6160" max="6160" width="11.6484375" customWidth="1"/>
+    <col min="6161" max="6161" width="12.34765625" customWidth="1"/>
+    <col min="6403" max="6403" width="56.6484375" customWidth="1"/>
+    <col min="6404" max="6404" width="14.1484375" customWidth="1"/>
+    <col min="6405" max="6405" width="13.1484375" customWidth="1"/>
+    <col min="6406" max="6406" width="12.84765625" customWidth="1"/>
+    <col min="6407" max="6407" width="13.6484375" customWidth="1"/>
     <col min="6408" max="6409" width="13" customWidth="1"/>
-    <col min="6410" max="6410" width="12.6640625" customWidth="1"/>
-    <col min="6411" max="6411" width="11.33203125" customWidth="1"/>
-    <col min="6412" max="6412" width="12.33203125" customWidth="1"/>
+    <col min="6410" max="6410" width="12.6484375" customWidth="1"/>
+    <col min="6411" max="6411" width="11.34765625" customWidth="1"/>
+    <col min="6412" max="6412" width="12.34765625" customWidth="1"/>
     <col min="6413" max="6413" width="13" customWidth="1"/>
-    <col min="6414" max="6414" width="11.83203125" customWidth="1"/>
-    <col min="6415" max="6415" width="12.1640625" customWidth="1"/>
-    <col min="6416" max="6416" width="11.6640625" customWidth="1"/>
-    <col min="6417" max="6417" width="12.33203125" customWidth="1"/>
-    <col min="6659" max="6659" width="56.6640625" customWidth="1"/>
-    <col min="6660" max="6660" width="14.1640625" customWidth="1"/>
-    <col min="6661" max="6661" width="13.1640625" customWidth="1"/>
-    <col min="6662" max="6662" width="12.83203125" customWidth="1"/>
-    <col min="6663" max="6663" width="13.6640625" customWidth="1"/>
+    <col min="6414" max="6414" width="11.84765625" customWidth="1"/>
+    <col min="6415" max="6415" width="12.1484375" customWidth="1"/>
+    <col min="6416" max="6416" width="11.6484375" customWidth="1"/>
+    <col min="6417" max="6417" width="12.34765625" customWidth="1"/>
+    <col min="6659" max="6659" width="56.6484375" customWidth="1"/>
+    <col min="6660" max="6660" width="14.1484375" customWidth="1"/>
+    <col min="6661" max="6661" width="13.1484375" customWidth="1"/>
+    <col min="6662" max="6662" width="12.84765625" customWidth="1"/>
+    <col min="6663" max="6663" width="13.6484375" customWidth="1"/>
     <col min="6664" max="6665" width="13" customWidth="1"/>
-    <col min="6666" max="6666" width="12.6640625" customWidth="1"/>
-    <col min="6667" max="6667" width="11.33203125" customWidth="1"/>
-    <col min="6668" max="6668" width="12.33203125" customWidth="1"/>
+    <col min="6666" max="6666" width="12.6484375" customWidth="1"/>
+    <col min="6667" max="6667" width="11.34765625" customWidth="1"/>
+    <col min="6668" max="6668" width="12.34765625" customWidth="1"/>
     <col min="6669" max="6669" width="13" customWidth="1"/>
-    <col min="6670" max="6670" width="11.83203125" customWidth="1"/>
-    <col min="6671" max="6671" width="12.1640625" customWidth="1"/>
-    <col min="6672" max="6672" width="11.6640625" customWidth="1"/>
-    <col min="6673" max="6673" width="12.33203125" customWidth="1"/>
-    <col min="6915" max="6915" width="56.6640625" customWidth="1"/>
-    <col min="6916" max="6916" width="14.1640625" customWidth="1"/>
-    <col min="6917" max="6917" width="13.1640625" customWidth="1"/>
-    <col min="6918" max="6918" width="12.83203125" customWidth="1"/>
-    <col min="6919" max="6919" width="13.6640625" customWidth="1"/>
+    <col min="6670" max="6670" width="11.84765625" customWidth="1"/>
+    <col min="6671" max="6671" width="12.1484375" customWidth="1"/>
+    <col min="6672" max="6672" width="11.6484375" customWidth="1"/>
+    <col min="6673" max="6673" width="12.34765625" customWidth="1"/>
+    <col min="6915" max="6915" width="56.6484375" customWidth="1"/>
+    <col min="6916" max="6916" width="14.1484375" customWidth="1"/>
+    <col min="6917" max="6917" width="13.1484375" customWidth="1"/>
+    <col min="6918" max="6918" width="12.84765625" customWidth="1"/>
+    <col min="6919" max="6919" width="13.6484375" customWidth="1"/>
     <col min="6920" max="6921" width="13" customWidth="1"/>
-    <col min="6922" max="6922" width="12.6640625" customWidth="1"/>
-    <col min="6923" max="6923" width="11.33203125" customWidth="1"/>
-    <col min="6924" max="6924" width="12.33203125" customWidth="1"/>
+    <col min="6922" max="6922" width="12.6484375" customWidth="1"/>
+    <col min="6923" max="6923" width="11.34765625" customWidth="1"/>
+    <col min="6924" max="6924" width="12.34765625" customWidth="1"/>
     <col min="6925" max="6925" width="13" customWidth="1"/>
-    <col min="6926" max="6926" width="11.83203125" customWidth="1"/>
-    <col min="6927" max="6927" width="12.1640625" customWidth="1"/>
-    <col min="6928" max="6928" width="11.6640625" customWidth="1"/>
-    <col min="6929" max="6929" width="12.33203125" customWidth="1"/>
-    <col min="7171" max="7171" width="56.6640625" customWidth="1"/>
-    <col min="7172" max="7172" width="14.1640625" customWidth="1"/>
-    <col min="7173" max="7173" width="13.1640625" customWidth="1"/>
-    <col min="7174" max="7174" width="12.83203125" customWidth="1"/>
-    <col min="7175" max="7175" width="13.6640625" customWidth="1"/>
+    <col min="6926" max="6926" width="11.84765625" customWidth="1"/>
+    <col min="6927" max="6927" width="12.1484375" customWidth="1"/>
+    <col min="6928" max="6928" width="11.6484375" customWidth="1"/>
+    <col min="6929" max="6929" width="12.34765625" customWidth="1"/>
+    <col min="7171" max="7171" width="56.6484375" customWidth="1"/>
+    <col min="7172" max="7172" width="14.1484375" customWidth="1"/>
+    <col min="7173" max="7173" width="13.1484375" customWidth="1"/>
+    <col min="7174" max="7174" width="12.84765625" customWidth="1"/>
+    <col min="7175" max="7175" width="13.6484375" customWidth="1"/>
     <col min="7176" max="7177" width="13" customWidth="1"/>
-    <col min="7178" max="7178" width="12.6640625" customWidth="1"/>
-    <col min="7179" max="7179" width="11.33203125" customWidth="1"/>
-    <col min="7180" max="7180" width="12.33203125" customWidth="1"/>
+    <col min="7178" max="7178" width="12.6484375" customWidth="1"/>
+    <col min="7179" max="7179" width="11.34765625" customWidth="1"/>
+    <col min="7180" max="7180" width="12.34765625" customWidth="1"/>
     <col min="7181" max="7181" width="13" customWidth="1"/>
-    <col min="7182" max="7182" width="11.83203125" customWidth="1"/>
-    <col min="7183" max="7183" width="12.1640625" customWidth="1"/>
-    <col min="7184" max="7184" width="11.6640625" customWidth="1"/>
-    <col min="7185" max="7185" width="12.33203125" customWidth="1"/>
-    <col min="7427" max="7427" width="56.6640625" customWidth="1"/>
-    <col min="7428" max="7428" width="14.1640625" customWidth="1"/>
-    <col min="7429" max="7429" width="13.1640625" customWidth="1"/>
-    <col min="7430" max="7430" width="12.83203125" customWidth="1"/>
-    <col min="7431" max="7431" width="13.6640625" customWidth="1"/>
+    <col min="7182" max="7182" width="11.84765625" customWidth="1"/>
+    <col min="7183" max="7183" width="12.1484375" customWidth="1"/>
+    <col min="7184" max="7184" width="11.6484375" customWidth="1"/>
+    <col min="7185" max="7185" width="12.34765625" customWidth="1"/>
+    <col min="7427" max="7427" width="56.6484375" customWidth="1"/>
+    <col min="7428" max="7428" width="14.1484375" customWidth="1"/>
+    <col min="7429" max="7429" width="13.1484375" customWidth="1"/>
+    <col min="7430" max="7430" width="12.84765625" customWidth="1"/>
+    <col min="7431" max="7431" width="13.6484375" customWidth="1"/>
     <col min="7432" max="7433" width="13" customWidth="1"/>
-    <col min="7434" max="7434" width="12.6640625" customWidth="1"/>
-    <col min="7435" max="7435" width="11.33203125" customWidth="1"/>
-    <col min="7436" max="7436" width="12.33203125" customWidth="1"/>
+    <col min="7434" max="7434" width="12.6484375" customWidth="1"/>
+    <col min="7435" max="7435" width="11.34765625" customWidth="1"/>
+    <col min="7436" max="7436" width="12.34765625" customWidth="1"/>
     <col min="7437" max="7437" width="13" customWidth="1"/>
-    <col min="7438" max="7438" width="11.83203125" customWidth="1"/>
-    <col min="7439" max="7439" width="12.1640625" customWidth="1"/>
-    <col min="7440" max="7440" width="11.6640625" customWidth="1"/>
-    <col min="7441" max="7441" width="12.33203125" customWidth="1"/>
-    <col min="7683" max="7683" width="56.6640625" customWidth="1"/>
-    <col min="7684" max="7684" width="14.1640625" customWidth="1"/>
-    <col min="7685" max="7685" width="13.1640625" customWidth="1"/>
-    <col min="7686" max="7686" width="12.83203125" customWidth="1"/>
-    <col min="7687" max="7687" width="13.6640625" customWidth="1"/>
+    <col min="7438" max="7438" width="11.84765625" customWidth="1"/>
+    <col min="7439" max="7439" width="12.1484375" customWidth="1"/>
+    <col min="7440" max="7440" width="11.6484375" customWidth="1"/>
+    <col min="7441" max="7441" width="12.34765625" customWidth="1"/>
+    <col min="7683" max="7683" width="56.6484375" customWidth="1"/>
+    <col min="7684" max="7684" width="14.1484375" customWidth="1"/>
+    <col min="7685" max="7685" width="13.1484375" customWidth="1"/>
+    <col min="7686" max="7686" width="12.84765625" customWidth="1"/>
+    <col min="7687" max="7687" width="13.6484375" customWidth="1"/>
     <col min="7688" max="7689" width="13" customWidth="1"/>
-    <col min="7690" max="7690" width="12.6640625" customWidth="1"/>
-    <col min="7691" max="7691" width="11.33203125" customWidth="1"/>
-    <col min="7692" max="7692" width="12.33203125" customWidth="1"/>
+    <col min="7690" max="7690" width="12.6484375" customWidth="1"/>
+    <col min="7691" max="7691" width="11.34765625" customWidth="1"/>
+    <col min="7692" max="7692" width="12.34765625" customWidth="1"/>
     <col min="7693" max="7693" width="13" customWidth="1"/>
-    <col min="7694" max="7694" width="11.83203125" customWidth="1"/>
-    <col min="7695" max="7695" width="12.1640625" customWidth="1"/>
-    <col min="7696" max="7696" width="11.6640625" customWidth="1"/>
-    <col min="7697" max="7697" width="12.33203125" customWidth="1"/>
-    <col min="7939" max="7939" width="56.6640625" customWidth="1"/>
-    <col min="7940" max="7940" width="14.1640625" customWidth="1"/>
-    <col min="7941" max="7941" width="13.1640625" customWidth="1"/>
-    <col min="7942" max="7942" width="12.83203125" customWidth="1"/>
-    <col min="7943" max="7943" width="13.6640625" customWidth="1"/>
+    <col min="7694" max="7694" width="11.84765625" customWidth="1"/>
+    <col min="7695" max="7695" width="12.1484375" customWidth="1"/>
+    <col min="7696" max="7696" width="11.6484375" customWidth="1"/>
+    <col min="7697" max="7697" width="12.34765625" customWidth="1"/>
+    <col min="7939" max="7939" width="56.6484375" customWidth="1"/>
+    <col min="7940" max="7940" width="14.1484375" customWidth="1"/>
+    <col min="7941" max="7941" width="13.1484375" customWidth="1"/>
+    <col min="7942" max="7942" width="12.84765625" customWidth="1"/>
+    <col min="7943" max="7943" width="13.6484375" customWidth="1"/>
     <col min="7944" max="7945" width="13" customWidth="1"/>
-    <col min="7946" max="7946" width="12.6640625" customWidth="1"/>
-    <col min="7947" max="7947" width="11.33203125" customWidth="1"/>
-    <col min="7948" max="7948" width="12.33203125" customWidth="1"/>
+    <col min="7946" max="7946" width="12.6484375" customWidth="1"/>
+    <col min="7947" max="7947" width="11.34765625" customWidth="1"/>
+    <col min="7948" max="7948" width="12.34765625" customWidth="1"/>
     <col min="7949" max="7949" width="13" customWidth="1"/>
-    <col min="7950" max="7950" width="11.83203125" customWidth="1"/>
-    <col min="7951" max="7951" width="12.1640625" customWidth="1"/>
-    <col min="7952" max="7952" width="11.6640625" customWidth="1"/>
-    <col min="7953" max="7953" width="12.33203125" customWidth="1"/>
-    <col min="8195" max="8195" width="56.6640625" customWidth="1"/>
-    <col min="8196" max="8196" width="14.1640625" customWidth="1"/>
-    <col min="8197" max="8197" width="13.1640625" customWidth="1"/>
-    <col min="8198" max="8198" width="12.83203125" customWidth="1"/>
-    <col min="8199" max="8199" width="13.6640625" customWidth="1"/>
+    <col min="7950" max="7950" width="11.84765625" customWidth="1"/>
+    <col min="7951" max="7951" width="12.1484375" customWidth="1"/>
+    <col min="7952" max="7952" width="11.6484375" customWidth="1"/>
+    <col min="7953" max="7953" width="12.34765625" customWidth="1"/>
+    <col min="8195" max="8195" width="56.6484375" customWidth="1"/>
+    <col min="8196" max="8196" width="14.1484375" customWidth="1"/>
+    <col min="8197" max="8197" width="13.1484375" customWidth="1"/>
+    <col min="8198" max="8198" width="12.84765625" customWidth="1"/>
+    <col min="8199" max="8199" width="13.6484375" customWidth="1"/>
     <col min="8200" max="8201" width="13" customWidth="1"/>
-    <col min="8202" max="8202" width="12.6640625" customWidth="1"/>
-    <col min="8203" max="8203" width="11.33203125" customWidth="1"/>
-    <col min="8204" max="8204" width="12.33203125" customWidth="1"/>
+    <col min="8202" max="8202" width="12.6484375" customWidth="1"/>
+    <col min="8203" max="8203" width="11.34765625" customWidth="1"/>
+    <col min="8204" max="8204" width="12.34765625" customWidth="1"/>
     <col min="8205" max="8205" width="13" customWidth="1"/>
-    <col min="8206" max="8206" width="11.83203125" customWidth="1"/>
-    <col min="8207" max="8207" width="12.1640625" customWidth="1"/>
-    <col min="8208" max="8208" width="11.6640625" customWidth="1"/>
-    <col min="8209" max="8209" width="12.33203125" customWidth="1"/>
-    <col min="8451" max="8451" width="56.6640625" customWidth="1"/>
-    <col min="8452" max="8452" width="14.1640625" customWidth="1"/>
-    <col min="8453" max="8453" width="13.1640625" customWidth="1"/>
-    <col min="8454" max="8454" width="12.83203125" customWidth="1"/>
-    <col min="8455" max="8455" width="13.6640625" customWidth="1"/>
+    <col min="8206" max="8206" width="11.84765625" customWidth="1"/>
+    <col min="8207" max="8207" width="12.1484375" customWidth="1"/>
+    <col min="8208" max="8208" width="11.6484375" customWidth="1"/>
+    <col min="8209" max="8209" width="12.34765625" customWidth="1"/>
+    <col min="8451" max="8451" width="56.6484375" customWidth="1"/>
+    <col min="8452" max="8452" width="14.1484375" customWidth="1"/>
+    <col min="8453" max="8453" width="13.1484375" customWidth="1"/>
+    <col min="8454" max="8454" width="12.84765625" customWidth="1"/>
+    <col min="8455" max="8455" width="13.6484375" customWidth="1"/>
     <col min="8456" max="8457" width="13" customWidth="1"/>
-    <col min="8458" max="8458" width="12.6640625" customWidth="1"/>
-    <col min="8459" max="8459" width="11.33203125" customWidth="1"/>
-    <col min="8460" max="8460" width="12.33203125" customWidth="1"/>
+    <col min="8458" max="8458" width="12.6484375" customWidth="1"/>
+    <col min="8459" max="8459" width="11.34765625" customWidth="1"/>
+    <col min="8460" max="8460" width="12.34765625" customWidth="1"/>
     <col min="8461" max="8461" width="13" customWidth="1"/>
-    <col min="8462" max="8462" width="11.83203125" customWidth="1"/>
-    <col min="8463" max="8463" width="12.1640625" customWidth="1"/>
-    <col min="8464" max="8464" width="11.6640625" customWidth="1"/>
-    <col min="8465" max="8465" width="12.33203125" customWidth="1"/>
-    <col min="8707" max="8707" width="56.6640625" customWidth="1"/>
-    <col min="8708" max="8708" width="14.1640625" customWidth="1"/>
-    <col min="8709" max="8709" width="13.1640625" customWidth="1"/>
-    <col min="8710" max="8710" width="12.83203125" customWidth="1"/>
-    <col min="8711" max="8711" width="13.6640625" customWidth="1"/>
+    <col min="8462" max="8462" width="11.84765625" customWidth="1"/>
+    <col min="8463" max="8463" width="12.1484375" customWidth="1"/>
+    <col min="8464" max="8464" width="11.6484375" customWidth="1"/>
+    <col min="8465" max="8465" width="12.34765625" customWidth="1"/>
+    <col min="8707" max="8707" width="56.6484375" customWidth="1"/>
+    <col min="8708" max="8708" width="14.1484375" customWidth="1"/>
+    <col min="8709" max="8709" width="13.1484375" customWidth="1"/>
+    <col min="8710" max="8710" width="12.84765625" customWidth="1"/>
+    <col min="8711" max="8711" width="13.6484375" customWidth="1"/>
     <col min="8712" max="8713" width="13" customWidth="1"/>
-    <col min="8714" max="8714" width="12.6640625" customWidth="1"/>
-    <col min="8715" max="8715" width="11.33203125" customWidth="1"/>
-    <col min="8716" max="8716" width="12.33203125" customWidth="1"/>
+    <col min="8714" max="8714" width="12.6484375" customWidth="1"/>
+    <col min="8715" max="8715" width="11.34765625" customWidth="1"/>
+    <col min="8716" max="8716" width="12.34765625" customWidth="1"/>
     <col min="8717" max="8717" width="13" customWidth="1"/>
-    <col min="8718" max="8718" width="11.83203125" customWidth="1"/>
-    <col min="8719" max="8719" width="12.1640625" customWidth="1"/>
-    <col min="8720" max="8720" width="11.6640625" customWidth="1"/>
-    <col min="8721" max="8721" width="12.33203125" customWidth="1"/>
-    <col min="8963" max="8963" width="56.6640625" customWidth="1"/>
-    <col min="8964" max="8964" width="14.1640625" customWidth="1"/>
-    <col min="8965" max="8965" width="13.1640625" customWidth="1"/>
-    <col min="8966" max="8966" width="12.83203125" customWidth="1"/>
-    <col min="8967" max="8967" width="13.6640625" customWidth="1"/>
+    <col min="8718" max="8718" width="11.84765625" customWidth="1"/>
+    <col min="8719" max="8719" width="12.1484375" customWidth="1"/>
+    <col min="8720" max="8720" width="11.6484375" customWidth="1"/>
+    <col min="8721" max="8721" width="12.34765625" customWidth="1"/>
+    <col min="8963" max="8963" width="56.6484375" customWidth="1"/>
+    <col min="8964" max="8964" width="14.1484375" customWidth="1"/>
+    <col min="8965" max="8965" width="13.1484375" customWidth="1"/>
+    <col min="8966" max="8966" width="12.84765625" customWidth="1"/>
+    <col min="8967" max="8967" width="13.6484375" customWidth="1"/>
     <col min="8968" max="8969" width="13" customWidth="1"/>
-    <col min="8970" max="8970" width="12.6640625" customWidth="1"/>
-    <col min="8971" max="8971" width="11.33203125" customWidth="1"/>
-    <col min="8972" max="8972" width="12.33203125" customWidth="1"/>
+    <col min="8970" max="8970" width="12.6484375" customWidth="1"/>
+    <col min="8971" max="8971" width="11.34765625" customWidth="1"/>
+    <col min="8972" max="8972" width="12.34765625" customWidth="1"/>
     <col min="8973" max="8973" width="13" customWidth="1"/>
-    <col min="8974" max="8974" width="11.83203125" customWidth="1"/>
-    <col min="8975" max="8975" width="12.1640625" customWidth="1"/>
-    <col min="8976" max="8976" width="11.6640625" customWidth="1"/>
-    <col min="8977" max="8977" width="12.33203125" customWidth="1"/>
-    <col min="9219" max="9219" width="56.6640625" customWidth="1"/>
-    <col min="9220" max="9220" width="14.1640625" customWidth="1"/>
-    <col min="9221" max="9221" width="13.1640625" customWidth="1"/>
-    <col min="9222" max="9222" width="12.83203125" customWidth="1"/>
-    <col min="9223" max="9223" width="13.6640625" customWidth="1"/>
+    <col min="8974" max="8974" width="11.84765625" customWidth="1"/>
+    <col min="8975" max="8975" width="12.1484375" customWidth="1"/>
+    <col min="8976" max="8976" width="11.6484375" customWidth="1"/>
+    <col min="8977" max="8977" width="12.34765625" customWidth="1"/>
+    <col min="9219" max="9219" width="56.6484375" customWidth="1"/>
+    <col min="9220" max="9220" width="14.1484375" customWidth="1"/>
+    <col min="9221" max="9221" width="13.1484375" customWidth="1"/>
+    <col min="9222" max="9222" width="12.84765625" customWidth="1"/>
+    <col min="9223" max="9223" width="13.6484375" customWidth="1"/>
     <col min="9224" max="9225" width="13" customWidth="1"/>
-    <col min="9226" max="9226" width="12.6640625" customWidth="1"/>
-    <col min="9227" max="9227" width="11.33203125" customWidth="1"/>
-    <col min="9228" max="9228" width="12.33203125" customWidth="1"/>
+    <col min="9226" max="9226" width="12.6484375" customWidth="1"/>
+    <col min="9227" max="9227" width="11.34765625" customWidth="1"/>
+    <col min="9228" max="9228" width="12.34765625" customWidth="1"/>
     <col min="9229" max="9229" width="13" customWidth="1"/>
-    <col min="9230" max="9230" width="11.83203125" customWidth="1"/>
-    <col min="9231" max="9231" width="12.1640625" customWidth="1"/>
-    <col min="9232" max="9232" width="11.6640625" customWidth="1"/>
-    <col min="9233" max="9233" width="12.33203125" customWidth="1"/>
-    <col min="9475" max="9475" width="56.6640625" customWidth="1"/>
-    <col min="9476" max="9476" width="14.1640625" customWidth="1"/>
-    <col min="9477" max="9477" width="13.1640625" customWidth="1"/>
-    <col min="9478" max="9478" width="12.83203125" customWidth="1"/>
-    <col min="9479" max="9479" width="13.6640625" customWidth="1"/>
+    <col min="9230" max="9230" width="11.84765625" customWidth="1"/>
+    <col min="9231" max="9231" width="12.1484375" customWidth="1"/>
+    <col min="9232" max="9232" width="11.6484375" customWidth="1"/>
+    <col min="9233" max="9233" width="12.34765625" customWidth="1"/>
+    <col min="9475" max="9475" width="56.6484375" customWidth="1"/>
+    <col min="9476" max="9476" width="14.1484375" customWidth="1"/>
+    <col min="9477" max="9477" width="13.1484375" customWidth="1"/>
+    <col min="9478" max="9478" width="12.84765625" customWidth="1"/>
+    <col min="9479" max="9479" width="13.6484375" customWidth="1"/>
     <col min="9480" max="9481" width="13" customWidth="1"/>
-    <col min="9482" max="9482" width="12.6640625" customWidth="1"/>
-    <col min="9483" max="9483" width="11.33203125" customWidth="1"/>
-    <col min="9484" max="9484" width="12.33203125" customWidth="1"/>
+    <col min="9482" max="9482" width="12.6484375" customWidth="1"/>
+    <col min="9483" max="9483" width="11.34765625" customWidth="1"/>
+    <col min="9484" max="9484" width="12.34765625" customWidth="1"/>
     <col min="9485" max="9485" width="13" customWidth="1"/>
-    <col min="9486" max="9486" width="11.83203125" customWidth="1"/>
-    <col min="9487" max="9487" width="12.1640625" customWidth="1"/>
-    <col min="9488" max="9488" width="11.6640625" customWidth="1"/>
-    <col min="9489" max="9489" width="12.33203125" customWidth="1"/>
-    <col min="9731" max="9731" width="56.6640625" customWidth="1"/>
-    <col min="9732" max="9732" width="14.1640625" customWidth="1"/>
-    <col min="9733" max="9733" width="13.1640625" customWidth="1"/>
-    <col min="9734" max="9734" width="12.83203125" customWidth="1"/>
-    <col min="9735" max="9735" width="13.6640625" customWidth="1"/>
+    <col min="9486" max="9486" width="11.84765625" customWidth="1"/>
+    <col min="9487" max="9487" width="12.1484375" customWidth="1"/>
+    <col min="9488" max="9488" width="11.6484375" customWidth="1"/>
+    <col min="9489" max="9489" width="12.34765625" customWidth="1"/>
+    <col min="9731" max="9731" width="56.6484375" customWidth="1"/>
+    <col min="9732" max="9732" width="14.1484375" customWidth="1"/>
+    <col min="9733" max="9733" width="13.1484375" customWidth="1"/>
+    <col min="9734" max="9734" width="12.84765625" customWidth="1"/>
+    <col min="9735" max="9735" width="13.6484375" customWidth="1"/>
     <col min="9736" max="9737" width="13" customWidth="1"/>
-    <col min="9738" max="9738" width="12.6640625" customWidth="1"/>
-    <col min="9739" max="9739" width="11.33203125" customWidth="1"/>
-    <col min="9740" max="9740" width="12.33203125" customWidth="1"/>
+    <col min="9738" max="9738" width="12.6484375" customWidth="1"/>
+    <col min="9739" max="9739" width="11.34765625" customWidth="1"/>
+    <col min="9740" max="9740" width="12.34765625" customWidth="1"/>
     <col min="9741" max="9741" width="13" customWidth="1"/>
-    <col min="9742" max="9742" width="11.83203125" customWidth="1"/>
-    <col min="9743" max="9743" width="12.1640625" customWidth="1"/>
-    <col min="9744" max="9744" width="11.6640625" customWidth="1"/>
-    <col min="9745" max="9745" width="12.33203125" customWidth="1"/>
-    <col min="9987" max="9987" width="56.6640625" customWidth="1"/>
-    <col min="9988" max="9988" width="14.1640625" customWidth="1"/>
-    <col min="9989" max="9989" width="13.1640625" customWidth="1"/>
-    <col min="9990" max="9990" width="12.83203125" customWidth="1"/>
-    <col min="9991" max="9991" width="13.6640625" customWidth="1"/>
+    <col min="9742" max="9742" width="11.84765625" customWidth="1"/>
+    <col min="9743" max="9743" width="12.1484375" customWidth="1"/>
+    <col min="9744" max="9744" width="11.6484375" customWidth="1"/>
+    <col min="9745" max="9745" width="12.34765625" customWidth="1"/>
+    <col min="9987" max="9987" width="56.6484375" customWidth="1"/>
+    <col min="9988" max="9988" width="14.1484375" customWidth="1"/>
+    <col min="9989" max="9989" width="13.1484375" customWidth="1"/>
+    <col min="9990" max="9990" width="12.84765625" customWidth="1"/>
+    <col min="9991" max="9991" width="13.6484375" customWidth="1"/>
     <col min="9992" max="9993" width="13" customWidth="1"/>
-    <col min="9994" max="9994" width="12.6640625" customWidth="1"/>
-    <col min="9995" max="9995" width="11.33203125" customWidth="1"/>
-    <col min="9996" max="9996" width="12.33203125" customWidth="1"/>
+    <col min="9994" max="9994" width="12.6484375" customWidth="1"/>
+    <col min="9995" max="9995" width="11.34765625" customWidth="1"/>
+    <col min="9996" max="9996" width="12.34765625" customWidth="1"/>
     <col min="9997" max="9997" width="13" customWidth="1"/>
-    <col min="9998" max="9998" width="11.83203125" customWidth="1"/>
-    <col min="9999" max="9999" width="12.1640625" customWidth="1"/>
-    <col min="10000" max="10000" width="11.6640625" customWidth="1"/>
-    <col min="10001" max="10001" width="12.33203125" customWidth="1"/>
-    <col min="10243" max="10243" width="56.6640625" customWidth="1"/>
-    <col min="10244" max="10244" width="14.1640625" customWidth="1"/>
-    <col min="10245" max="10245" width="13.1640625" customWidth="1"/>
-    <col min="10246" max="10246" width="12.83203125" customWidth="1"/>
-    <col min="10247" max="10247" width="13.6640625" customWidth="1"/>
+    <col min="9998" max="9998" width="11.84765625" customWidth="1"/>
+    <col min="9999" max="9999" width="12.1484375" customWidth="1"/>
+    <col min="10000" max="10000" width="11.6484375" customWidth="1"/>
+    <col min="10001" max="10001" width="12.34765625" customWidth="1"/>
+    <col min="10243" max="10243" width="56.6484375" customWidth="1"/>
+    <col min="10244" max="10244" width="14.1484375" customWidth="1"/>
+    <col min="10245" max="10245" width="13.1484375" customWidth="1"/>
+    <col min="10246" max="10246" width="12.84765625" customWidth="1"/>
+    <col min="10247" max="10247" width="13.6484375" customWidth="1"/>
     <col min="10248" max="10249" width="13" customWidth="1"/>
-    <col min="10250" max="10250" width="12.6640625" customWidth="1"/>
-    <col min="10251" max="10251" width="11.33203125" customWidth="1"/>
-    <col min="10252" max="10252" width="12.33203125" customWidth="1"/>
+    <col min="10250" max="10250" width="12.6484375" customWidth="1"/>
+    <col min="10251" max="10251" width="11.34765625" customWidth="1"/>
+    <col min="10252" max="10252" width="12.34765625" customWidth="1"/>
     <col min="10253" max="10253" width="13" customWidth="1"/>
-    <col min="10254" max="10254" width="11.83203125" customWidth="1"/>
-    <col min="10255" max="10255" width="12.1640625" customWidth="1"/>
-    <col min="10256" max="10256" width="11.6640625" customWidth="1"/>
-    <col min="10257" max="10257" width="12.33203125" customWidth="1"/>
-    <col min="10499" max="10499" width="56.6640625" customWidth="1"/>
-    <col min="10500" max="10500" width="14.1640625" customWidth="1"/>
-    <col min="10501" max="10501" width="13.1640625" customWidth="1"/>
-    <col min="10502" max="10502" width="12.83203125" customWidth="1"/>
-    <col min="10503" max="10503" width="13.6640625" customWidth="1"/>
+    <col min="10254" max="10254" width="11.84765625" customWidth="1"/>
+    <col min="10255" max="10255" width="12.1484375" customWidth="1"/>
+    <col min="10256" max="10256" width="11.6484375" customWidth="1"/>
+    <col min="10257" max="10257" width="12.34765625" customWidth="1"/>
+    <col min="10499" max="10499" width="56.6484375" customWidth="1"/>
+    <col min="10500" max="10500" width="14.1484375" customWidth="1"/>
+    <col min="10501" max="10501" width="13.1484375" customWidth="1"/>
+    <col min="10502" max="10502" width="12.84765625" customWidth="1"/>
+    <col min="10503" max="10503" width="13.6484375" customWidth="1"/>
     <col min="10504" max="10505" width="13" customWidth="1"/>
-    <col min="10506" max="10506" width="12.6640625" customWidth="1"/>
-    <col min="10507" max="10507" width="11.33203125" customWidth="1"/>
-    <col min="10508" max="10508" width="12.33203125" customWidth="1"/>
+    <col min="10506" max="10506" width="12.6484375" customWidth="1"/>
+    <col min="10507" max="10507" width="11.34765625" customWidth="1"/>
+    <col min="10508" max="10508" width="12.34765625" customWidth="1"/>
     <col min="10509" max="10509" width="13" customWidth="1"/>
-    <col min="10510" max="10510" width="11.83203125" customWidth="1"/>
-    <col min="10511" max="10511" width="12.1640625" customWidth="1"/>
-    <col min="10512" max="10512" width="11.6640625" customWidth="1"/>
-    <col min="10513" max="10513" width="12.33203125" customWidth="1"/>
-    <col min="10755" max="10755" width="56.6640625" customWidth="1"/>
-    <col min="10756" max="10756" width="14.1640625" customWidth="1"/>
-    <col min="10757" max="10757" width="13.1640625" customWidth="1"/>
-    <col min="10758" max="10758" width="12.83203125" customWidth="1"/>
-    <col min="10759" max="10759" width="13.6640625" customWidth="1"/>
+    <col min="10510" max="10510" width="11.84765625" customWidth="1"/>
+    <col min="10511" max="10511" width="12.1484375" customWidth="1"/>
+    <col min="10512" max="10512" width="11.6484375" customWidth="1"/>
+    <col min="10513" max="10513" width="12.34765625" customWidth="1"/>
+    <col min="10755" max="10755" width="56.6484375" customWidth="1"/>
+    <col min="10756" max="10756" width="14.1484375" customWidth="1"/>
+    <col min="10757" max="10757" width="13.1484375" customWidth="1"/>
+    <col min="10758" max="10758" width="12.84765625" customWidth="1"/>
+    <col min="10759" max="10759" width="13.6484375" customWidth="1"/>
     <col min="10760" max="10761" width="13" customWidth="1"/>
-    <col min="10762" max="10762" width="12.6640625" customWidth="1"/>
-    <col min="10763" max="10763" width="11.33203125" customWidth="1"/>
-    <col min="10764" max="10764" width="12.33203125" customWidth="1"/>
+    <col min="10762" max="10762" width="12.6484375" customWidth="1"/>
+    <col min="10763" max="10763" width="11.34765625" customWidth="1"/>
+    <col min="10764" max="10764" width="12.34765625" customWidth="1"/>
     <col min="10765" max="10765" width="13" customWidth="1"/>
-    <col min="10766" max="10766" width="11.83203125" customWidth="1"/>
-    <col min="10767" max="10767" width="12.1640625" customWidth="1"/>
-    <col min="10768" max="10768" width="11.6640625" customWidth="1"/>
-    <col min="10769" max="10769" width="12.33203125" customWidth="1"/>
-    <col min="11011" max="11011" width="56.6640625" customWidth="1"/>
-    <col min="11012" max="11012" width="14.1640625" customWidth="1"/>
-    <col min="11013" max="11013" width="13.1640625" customWidth="1"/>
-    <col min="11014" max="11014" width="12.83203125" customWidth="1"/>
-    <col min="11015" max="11015" width="13.6640625" customWidth="1"/>
+    <col min="10766" max="10766" width="11.84765625" customWidth="1"/>
+    <col min="10767" max="10767" width="12.1484375" customWidth="1"/>
+    <col min="10768" max="10768" width="11.6484375" customWidth="1"/>
+    <col min="10769" max="10769" width="12.34765625" customWidth="1"/>
+    <col min="11011" max="11011" width="56.6484375" customWidth="1"/>
+    <col min="11012" max="11012" width="14.1484375" customWidth="1"/>
+    <col min="11013" max="11013" width="13.1484375" customWidth="1"/>
+    <col min="11014" max="11014" width="12.84765625" customWidth="1"/>
+    <col min="11015" max="11015" width="13.6484375" customWidth="1"/>
     <col min="11016" max="11017" width="13" customWidth="1"/>
-    <col min="11018" max="11018" width="12.6640625" customWidth="1"/>
-    <col min="11019" max="11019" width="11.33203125" customWidth="1"/>
-    <col min="11020" max="11020" width="12.33203125" customWidth="1"/>
+    <col min="11018" max="11018" width="12.6484375" customWidth="1"/>
+    <col min="11019" max="11019" width="11.34765625" customWidth="1"/>
+    <col min="11020" max="11020" width="12.34765625" customWidth="1"/>
     <col min="11021" max="11021" width="13" customWidth="1"/>
-    <col min="11022" max="11022" width="11.83203125" customWidth="1"/>
-    <col min="11023" max="11023" width="12.1640625" customWidth="1"/>
-    <col min="11024" max="11024" width="11.6640625" customWidth="1"/>
-    <col min="11025" max="11025" width="12.33203125" customWidth="1"/>
-    <col min="11267" max="11267" width="56.6640625" customWidth="1"/>
-    <col min="11268" max="11268" width="14.1640625" customWidth="1"/>
-    <col min="11269" max="11269" width="13.1640625" customWidth="1"/>
-    <col min="11270" max="11270" width="12.83203125" customWidth="1"/>
-    <col min="11271" max="11271" width="13.6640625" customWidth="1"/>
+    <col min="11022" max="11022" width="11.84765625" customWidth="1"/>
+    <col min="11023" max="11023" width="12.1484375" customWidth="1"/>
+    <col min="11024" max="11024" width="11.6484375" customWidth="1"/>
+    <col min="11025" max="11025" width="12.34765625" customWidth="1"/>
+    <col min="11267" max="11267" width="56.6484375" customWidth="1"/>
+    <col min="11268" max="11268" width="14.1484375" customWidth="1"/>
+    <col min="11269" max="11269" width="13.1484375" customWidth="1"/>
+    <col min="11270" max="11270" width="12.84765625" customWidth="1"/>
+    <col min="11271" max="11271" width="13.6484375" customWidth="1"/>
     <col min="11272" max="11273" width="13" customWidth="1"/>
-    <col min="11274" max="11274" width="12.6640625" customWidth="1"/>
-    <col min="11275" max="11275" width="11.33203125" customWidth="1"/>
-    <col min="11276" max="11276" width="12.33203125" customWidth="1"/>
+    <col min="11274" max="11274" width="12.6484375" customWidth="1"/>
+    <col min="11275" max="11275" width="11.34765625" customWidth="1"/>
+    <col min="11276" max="11276" width="12.34765625" customWidth="1"/>
     <col min="11277" max="11277" width="13" customWidth="1"/>
-    <col min="11278" max="11278" width="11.83203125" customWidth="1"/>
-    <col min="11279" max="11279" width="12.1640625" customWidth="1"/>
-    <col min="11280" max="11280" width="11.6640625" customWidth="1"/>
-    <col min="11281" max="11281" width="12.33203125" customWidth="1"/>
-    <col min="11523" max="11523" width="56.6640625" customWidth="1"/>
-    <col min="11524" max="11524" width="14.1640625" customWidth="1"/>
-    <col min="11525" max="11525" width="13.1640625" customWidth="1"/>
-    <col min="11526" max="11526" width="12.83203125" customWidth="1"/>
-    <col min="11527" max="11527" width="13.6640625" customWidth="1"/>
+    <col min="11278" max="11278" width="11.84765625" customWidth="1"/>
+    <col min="11279" max="11279" width="12.1484375" customWidth="1"/>
+    <col min="11280" max="11280" width="11.6484375" customWidth="1"/>
+    <col min="11281" max="11281" width="12.34765625" customWidth="1"/>
+    <col min="11523" max="11523" width="56.6484375" customWidth="1"/>
+    <col min="11524" max="11524" width="14.1484375" customWidth="1"/>
+    <col min="11525" max="11525" width="13.1484375" customWidth="1"/>
+    <col min="11526" max="11526" width="12.84765625" customWidth="1"/>
+    <col min="11527" max="11527" width="13.6484375" customWidth="1"/>
     <col min="11528" max="11529" width="13" customWidth="1"/>
-    <col min="11530" max="11530" width="12.6640625" customWidth="1"/>
-    <col min="11531" max="11531" width="11.33203125" customWidth="1"/>
-    <col min="11532" max="11532" width="12.33203125" customWidth="1"/>
+    <col min="11530" max="11530" width="12.6484375" customWidth="1"/>
+    <col min="11531" max="11531" width="11.34765625" customWidth="1"/>
+    <col min="11532" max="11532" width="12.34765625" customWidth="1"/>
     <col min="11533" max="11533" width="13" customWidth="1"/>
-    <col min="11534" max="11534" width="11.83203125" customWidth="1"/>
-    <col min="11535" max="11535" width="12.1640625" customWidth="1"/>
-    <col min="11536" max="11536" width="11.6640625" customWidth="1"/>
-    <col min="11537" max="11537" width="12.33203125" customWidth="1"/>
-    <col min="11779" max="11779" width="56.6640625" customWidth="1"/>
-    <col min="11780" max="11780" width="14.1640625" customWidth="1"/>
-    <col min="11781" max="11781" width="13.1640625" customWidth="1"/>
-    <col min="11782" max="11782" width="12.83203125" customWidth="1"/>
-    <col min="11783" max="11783" width="13.6640625" customWidth="1"/>
+    <col min="11534" max="11534" width="11.84765625" customWidth="1"/>
+    <col min="11535" max="11535" width="12.1484375" customWidth="1"/>
+    <col min="11536" max="11536" width="11.6484375" customWidth="1"/>
+    <col min="11537" max="11537" width="12.34765625" customWidth="1"/>
+    <col min="11779" max="11779" width="56.6484375" customWidth="1"/>
+    <col min="11780" max="11780" width="14.1484375" customWidth="1"/>
+    <col min="11781" max="11781" width="13.1484375" customWidth="1"/>
+    <col min="11782" max="11782" width="12.84765625" customWidth="1"/>
+    <col min="11783" max="11783" width="13.6484375" customWidth="1"/>
     <col min="11784" max="11785" width="13" customWidth="1"/>
-    <col min="11786" max="11786" width="12.6640625" customWidth="1"/>
-    <col min="11787" max="11787" width="11.33203125" customWidth="1"/>
-    <col min="11788" max="11788" width="12.33203125" customWidth="1"/>
+    <col min="11786" max="11786" width="12.6484375" customWidth="1"/>
+    <col min="11787" max="11787" width="11.34765625" customWidth="1"/>
+    <col min="11788" max="11788" width="12.34765625" customWidth="1"/>
     <col min="11789" max="11789" width="13" customWidth="1"/>
-    <col min="11790" max="11790" width="11.83203125" customWidth="1"/>
-    <col min="11791" max="11791" width="12.1640625" customWidth="1"/>
-    <col min="11792" max="11792" width="11.6640625" customWidth="1"/>
-    <col min="11793" max="11793" width="12.33203125" customWidth="1"/>
-    <col min="12035" max="12035" width="56.6640625" customWidth="1"/>
-    <col min="12036" max="12036" width="14.1640625" customWidth="1"/>
-    <col min="12037" max="12037" width="13.1640625" customWidth="1"/>
-    <col min="12038" max="12038" width="12.83203125" customWidth="1"/>
-    <col min="12039" max="12039" width="13.6640625" customWidth="1"/>
+    <col min="11790" max="11790" width="11.84765625" customWidth="1"/>
+    <col min="11791" max="11791" width="12.1484375" customWidth="1"/>
+    <col min="11792" max="11792" width="11.6484375" customWidth="1"/>
+    <col min="11793" max="11793" width="12.34765625" customWidth="1"/>
+    <col min="12035" max="12035" width="56.6484375" customWidth="1"/>
+    <col min="12036" max="12036" width="14.1484375" customWidth="1"/>
+    <col min="12037" max="12037" width="13.1484375" customWidth="1"/>
+    <col min="12038" max="12038" width="12.84765625" customWidth="1"/>
+    <col min="12039" max="12039" width="13.6484375" customWidth="1"/>
     <col min="12040" max="12041" width="13" customWidth="1"/>
-    <col min="12042" max="12042" width="12.6640625" customWidth="1"/>
-    <col min="12043" max="12043" width="11.33203125" customWidth="1"/>
-    <col min="12044" max="12044" width="12.33203125" customWidth="1"/>
+    <col min="12042" max="12042" width="12.6484375" customWidth="1"/>
+    <col min="12043" max="12043" width="11.34765625" customWidth="1"/>
+    <col min="12044" max="12044" width="12.34765625" customWidth="1"/>
     <col min="12045" max="12045" width="13" customWidth="1"/>
-    <col min="12046" max="12046" width="11.83203125" customWidth="1"/>
-    <col min="12047" max="12047" width="12.1640625" customWidth="1"/>
-    <col min="12048" max="12048" width="11.6640625" customWidth="1"/>
-    <col min="12049" max="12049" width="12.33203125" customWidth="1"/>
-    <col min="12291" max="12291" width="56.6640625" customWidth="1"/>
-    <col min="12292" max="12292" width="14.1640625" customWidth="1"/>
-    <col min="12293" max="12293" width="13.1640625" customWidth="1"/>
-    <col min="12294" max="12294" width="12.83203125" customWidth="1"/>
-    <col min="12295" max="12295" width="13.6640625" customWidth="1"/>
+    <col min="12046" max="12046" width="11.84765625" customWidth="1"/>
+    <col min="12047" max="12047" width="12.1484375" customWidth="1"/>
+    <col min="12048" max="12048" width="11.6484375" customWidth="1"/>
+    <col min="12049" max="12049" width="12.34765625" customWidth="1"/>
+    <col min="12291" max="12291" width="56.6484375" customWidth="1"/>
+    <col min="12292" max="12292" width="14.1484375" customWidth="1"/>
+    <col min="12293" max="12293" width="13.1484375" customWidth="1"/>
+    <col min="12294" max="12294" width="12.84765625" customWidth="1"/>
+    <col min="12295" max="12295" width="13.6484375" customWidth="1"/>
     <col min="12296" max="12297" width="13" customWidth="1"/>
-    <col min="12298" max="12298" width="12.6640625" customWidth="1"/>
-    <col min="12299" max="12299" width="11.33203125" customWidth="1"/>
-    <col min="12300" max="12300" width="12.33203125" customWidth="1"/>
+    <col min="12298" max="12298" width="12.6484375" customWidth="1"/>
+    <col min="12299" max="12299" width="11.34765625" customWidth="1"/>
+    <col min="12300" max="12300" width="12.34765625" customWidth="1"/>
     <col min="12301" max="12301" width="13" customWidth="1"/>
-    <col min="12302" max="12302" width="11.83203125" customWidth="1"/>
-    <col min="12303" max="12303" width="12.1640625" customWidth="1"/>
-    <col min="12304" max="12304" width="11.6640625" customWidth="1"/>
-    <col min="12305" max="12305" width="12.33203125" customWidth="1"/>
-    <col min="12547" max="12547" width="56.6640625" customWidth="1"/>
-    <col min="12548" max="12548" width="14.1640625" customWidth="1"/>
-    <col min="12549" max="12549" width="13.1640625" customWidth="1"/>
-    <col min="12550" max="12550" width="12.83203125" customWidth="1"/>
-    <col min="12551" max="12551" width="13.6640625" customWidth="1"/>
+    <col min="12302" max="12302" width="11.84765625" customWidth="1"/>
+    <col min="12303" max="12303" width="12.1484375" customWidth="1"/>
+    <col min="12304" max="12304" width="11.6484375" customWidth="1"/>
+    <col min="12305" max="12305" width="12.34765625" customWidth="1"/>
+    <col min="12547" max="12547" width="56.6484375" customWidth="1"/>
+    <col min="12548" max="12548" width="14.1484375" customWidth="1"/>
+    <col min="12549" max="12549" width="13.1484375" customWidth="1"/>
+    <col min="12550" max="12550" width="12.84765625" customWidth="1"/>
+    <col min="12551" max="12551" width="13.6484375" customWidth="1"/>
     <col min="12552" max="12553" width="13" customWidth="1"/>
-    <col min="12554" max="12554" width="12.6640625" customWidth="1"/>
-    <col min="12555" max="12555" width="11.33203125" customWidth="1"/>
-    <col min="12556" max="12556" width="12.33203125" customWidth="1"/>
+    <col min="12554" max="12554" width="12.6484375" customWidth="1"/>
+    <col min="12555" max="12555" width="11.34765625" customWidth="1"/>
+    <col min="12556" max="12556" width="12.34765625" customWidth="1"/>
     <col min="12557" max="12557" width="13" customWidth="1"/>
-    <col min="12558" max="12558" width="11.83203125" customWidth="1"/>
-    <col min="12559" max="12559" width="12.1640625" customWidth="1"/>
-    <col min="12560" max="12560" width="11.6640625" customWidth="1"/>
-    <col min="12561" max="12561" width="12.33203125" customWidth="1"/>
-    <col min="12803" max="12803" width="56.6640625" customWidth="1"/>
-    <col min="12804" max="12804" width="14.1640625" customWidth="1"/>
-    <col min="12805" max="12805" width="13.1640625" customWidth="1"/>
-    <col min="12806" max="12806" width="12.83203125" customWidth="1"/>
-    <col min="12807" max="12807" width="13.6640625" customWidth="1"/>
+    <col min="12558" max="12558" width="11.84765625" customWidth="1"/>
+    <col min="12559" max="12559" width="12.1484375" customWidth="1"/>
+    <col min="12560" max="12560" width="11.6484375" customWidth="1"/>
+    <col min="12561" max="12561" width="12.34765625" customWidth="1"/>
+    <col min="12803" max="12803" width="56.6484375" customWidth="1"/>
+    <col min="12804" max="12804" width="14.1484375" customWidth="1"/>
+    <col min="12805" max="12805" width="13.1484375" customWidth="1"/>
+    <col min="12806" max="12806" width="12.84765625" customWidth="1"/>
+    <col min="12807" max="12807" width="13.6484375" customWidth="1"/>
     <col min="12808" max="12809" width="13" customWidth="1"/>
-    <col min="12810" max="12810" width="12.6640625" customWidth="1"/>
-    <col min="12811" max="12811" width="11.33203125" customWidth="1"/>
-    <col min="12812" max="12812" width="12.33203125" customWidth="1"/>
+    <col min="12810" max="12810" width="12.6484375" customWidth="1"/>
+    <col min="12811" max="12811" width="11.34765625" customWidth="1"/>
+    <col min="12812" max="12812" width="12.34765625" customWidth="1"/>
     <col min="12813" max="12813" width="13" customWidth="1"/>
-    <col min="12814" max="12814" width="11.83203125" customWidth="1"/>
-    <col min="12815" max="12815" width="12.1640625" customWidth="1"/>
-    <col min="12816" max="12816" width="11.6640625" customWidth="1"/>
-    <col min="12817" max="12817" width="12.33203125" customWidth="1"/>
-    <col min="13059" max="13059" width="56.6640625" customWidth="1"/>
-    <col min="13060" max="13060" width="14.1640625" customWidth="1"/>
-    <col min="13061" max="13061" width="13.1640625" customWidth="1"/>
-    <col min="13062" max="13062" width="12.83203125" customWidth="1"/>
-    <col min="13063" max="13063" width="13.6640625" customWidth="1"/>
+    <col min="12814" max="12814" width="11.84765625" customWidth="1"/>
+    <col min="12815" max="12815" width="12.1484375" customWidth="1"/>
+    <col min="12816" max="12816" width="11.6484375" customWidth="1"/>
+    <col min="12817" max="12817" width="12.34765625" customWidth="1"/>
+    <col min="13059" max="13059" width="56.6484375" customWidth="1"/>
+    <col min="13060" max="13060" width="14.1484375" customWidth="1"/>
+    <col min="13061" max="13061" width="13.1484375" customWidth="1"/>
+    <col min="13062" max="13062" width="12.84765625" customWidth="1"/>
+    <col min="13063" max="13063" width="13.6484375" customWidth="1"/>
     <col min="13064" max="13065" width="13" customWidth="1"/>
-    <col min="13066" max="13066" width="12.6640625" customWidth="1"/>
-    <col min="13067" max="13067" width="11.33203125" customWidth="1"/>
-    <col min="13068" max="13068" width="12.33203125" customWidth="1"/>
+    <col min="13066" max="13066" width="12.6484375" customWidth="1"/>
+    <col min="13067" max="13067" width="11.34765625" customWidth="1"/>
+    <col min="13068" max="13068" width="12.34765625" customWidth="1"/>
     <col min="13069" max="13069" width="13" customWidth="1"/>
-    <col min="13070" max="13070" width="11.83203125" customWidth="1"/>
-    <col min="13071" max="13071" width="12.1640625" customWidth="1"/>
-    <col min="13072" max="13072" width="11.6640625" customWidth="1"/>
-    <col min="13073" max="13073" width="12.33203125" customWidth="1"/>
-    <col min="13315" max="13315" width="56.6640625" customWidth="1"/>
-    <col min="13316" max="13316" width="14.1640625" customWidth="1"/>
-    <col min="13317" max="13317" width="13.1640625" customWidth="1"/>
-    <col min="13318" max="13318" width="12.83203125" customWidth="1"/>
-    <col min="13319" max="13319" width="13.6640625" customWidth="1"/>
+    <col min="13070" max="13070" width="11.84765625" customWidth="1"/>
+    <col min="13071" max="13071" width="12.1484375" customWidth="1"/>
+    <col min="13072" max="13072" width="11.6484375" customWidth="1"/>
+    <col min="13073" max="13073" width="12.34765625" customWidth="1"/>
+    <col min="13315" max="13315" width="56.6484375" customWidth="1"/>
+    <col min="13316" max="13316" width="14.1484375" customWidth="1"/>
+    <col min="13317" max="13317" width="13.1484375" customWidth="1"/>
+    <col min="13318" max="13318" width="12.84765625" customWidth="1"/>
+    <col min="13319" max="13319" width="13.6484375" customWidth="1"/>
     <col min="13320" max="13321" width="13" customWidth="1"/>
-    <col min="13322" max="13322" width="12.6640625" customWidth="1"/>
-    <col min="13323" max="13323" width="11.33203125" customWidth="1"/>
-    <col min="13324" max="13324" width="12.33203125" customWidth="1"/>
+    <col min="13322" max="13322" width="12.6484375" customWidth="1"/>
+    <col min="13323" max="13323" width="11.34765625" customWidth="1"/>
+    <col min="13324" max="13324" width="12.34765625" customWidth="1"/>
     <col min="13325" max="13325" width="13" customWidth="1"/>
-    <col min="13326" max="13326" width="11.83203125" customWidth="1"/>
-    <col min="13327" max="13327" width="12.1640625" customWidth="1"/>
-    <col min="13328" max="13328" width="11.6640625" customWidth="1"/>
-    <col min="13329" max="13329" width="12.33203125" customWidth="1"/>
-    <col min="13571" max="13571" width="56.6640625" customWidth="1"/>
-    <col min="13572" max="13572" width="14.1640625" customWidth="1"/>
-    <col min="13573" max="13573" width="13.1640625" customWidth="1"/>
-    <col min="13574" max="13574" width="12.83203125" customWidth="1"/>
-    <col min="13575" max="13575" width="13.6640625" customWidth="1"/>
+    <col min="13326" max="13326" width="11.84765625" customWidth="1"/>
+    <col min="13327" max="13327" width="12.1484375" customWidth="1"/>
+    <col min="13328" max="13328" width="11.6484375" customWidth="1"/>
+    <col min="13329" max="13329" width="12.34765625" customWidth="1"/>
+    <col min="13571" max="13571" width="56.6484375" customWidth="1"/>
+    <col min="13572" max="13572" width="14.1484375" customWidth="1"/>
+    <col min="13573" max="13573" width="13.1484375" customWidth="1"/>
+    <col min="13574" max="13574" width="12.84765625" customWidth="1"/>
+    <col min="13575" max="13575" width="13.6484375" customWidth="1"/>
     <col min="13576" max="13577" width="13" customWidth="1"/>
-    <col min="13578" max="13578" width="12.6640625" customWidth="1"/>
-    <col min="13579" max="13579" width="11.33203125" customWidth="1"/>
-    <col min="13580" max="13580" width="12.33203125" customWidth="1"/>
+    <col min="13578" max="13578" width="12.6484375" customWidth="1"/>
+    <col min="13579" max="13579" width="11.34765625" customWidth="1"/>
+    <col min="13580" max="13580" width="12.34765625" customWidth="1"/>
     <col min="13581" max="13581" width="13" customWidth="1"/>
-    <col min="13582" max="13582" width="11.83203125" customWidth="1"/>
-    <col min="13583" max="13583" width="12.1640625" customWidth="1"/>
-    <col min="13584" max="13584" width="11.6640625" customWidth="1"/>
-    <col min="13585" max="13585" width="12.33203125" customWidth="1"/>
-    <col min="13827" max="13827" width="56.6640625" customWidth="1"/>
-    <col min="13828" max="13828" width="14.1640625" customWidth="1"/>
-    <col min="13829" max="13829" width="13.1640625" customWidth="1"/>
-    <col min="13830" max="13830" width="12.83203125" customWidth="1"/>
-    <col min="13831" max="13831" width="13.6640625" customWidth="1"/>
+    <col min="13582" max="13582" width="11.84765625" customWidth="1"/>
+    <col min="13583" max="13583" width="12.1484375" customWidth="1"/>
+    <col min="13584" max="13584" width="11.6484375" customWidth="1"/>
+    <col min="13585" max="13585" width="12.34765625" customWidth="1"/>
+    <col min="13827" max="13827" width="56.6484375" customWidth="1"/>
+    <col min="13828" max="13828" width="14.1484375" customWidth="1"/>
+    <col min="13829" max="13829" width="13.1484375" customWidth="1"/>
+    <col min="13830" max="13830" width="12.84765625" customWidth="1"/>
+    <col min="13831" max="13831" width="13.6484375" customWidth="1"/>
     <col min="13832" max="13833" width="13" customWidth="1"/>
-    <col min="13834" max="13834" width="12.6640625" customWidth="1"/>
-    <col min="13835" max="13835" width="11.33203125" customWidth="1"/>
-    <col min="13836" max="13836" width="12.33203125" customWidth="1"/>
+    <col min="13834" max="13834" width="12.6484375" customWidth="1"/>
+    <col min="13835" max="13835" width="11.34765625" customWidth="1"/>
+    <col min="13836" max="13836" width="12.34765625" customWidth="1"/>
     <col min="13837" max="13837" width="13" customWidth="1"/>
-    <col min="13838" max="13838" width="11.83203125" customWidth="1"/>
-    <col min="13839" max="13839" width="12.1640625" customWidth="1"/>
-    <col min="13840" max="13840" width="11.6640625" customWidth="1"/>
-    <col min="13841" max="13841" width="12.33203125" customWidth="1"/>
-    <col min="14083" max="14083" width="56.6640625" customWidth="1"/>
-    <col min="14084" max="14084" width="14.1640625" customWidth="1"/>
-    <col min="14085" max="14085" width="13.1640625" customWidth="1"/>
-    <col min="14086" max="14086" width="12.83203125" customWidth="1"/>
-    <col min="14087" max="14087" width="13.6640625" customWidth="1"/>
+    <col min="13838" max="13838" width="11.84765625" customWidth="1"/>
+    <col min="13839" max="13839" width="12.1484375" customWidth="1"/>
+    <col min="13840" max="13840" width="11.6484375" customWidth="1"/>
+    <col min="13841" max="13841" width="12.34765625" customWidth="1"/>
+    <col min="14083" max="14083" width="56.6484375" customWidth="1"/>
+    <col min="14084" max="14084" width="14.1484375" customWidth="1"/>
+    <col min="14085" max="14085" width="13.1484375" customWidth="1"/>
+    <col min="14086" max="14086" width="12.84765625" customWidth="1"/>
+    <col min="14087" max="14087" width="13.6484375" customWidth="1"/>
     <col min="14088" max="14089" width="13" customWidth="1"/>
-    <col min="14090" max="14090" width="12.6640625" customWidth="1"/>
-    <col min="14091" max="14091" width="11.33203125" customWidth="1"/>
-    <col min="14092" max="14092" width="12.33203125" customWidth="1"/>
+    <col min="14090" max="14090" width="12.6484375" customWidth="1"/>
+    <col min="14091" max="14091" width="11.34765625" customWidth="1"/>
+    <col min="14092" max="14092" width="12.34765625" customWidth="1"/>
     <col min="14093" max="14093" width="13" customWidth="1"/>
-    <col min="14094" max="14094" width="11.83203125" customWidth="1"/>
-    <col min="14095" max="14095" width="12.1640625" customWidth="1"/>
-    <col min="14096" max="14096" width="11.6640625" customWidth="1"/>
-    <col min="14097" max="14097" width="12.33203125" customWidth="1"/>
-    <col min="14339" max="14339" width="56.6640625" customWidth="1"/>
-    <col min="14340" max="14340" width="14.1640625" customWidth="1"/>
-    <col min="14341" max="14341" width="13.1640625" customWidth="1"/>
-    <col min="14342" max="14342" width="12.83203125" customWidth="1"/>
-    <col min="14343" max="14343" width="13.6640625" customWidth="1"/>
+    <col min="14094" max="14094" width="11.84765625" customWidth="1"/>
+    <col min="14095" max="14095" width="12.1484375" customWidth="1"/>
+    <col min="14096" max="14096" width="11.6484375" customWidth="1"/>
+    <col min="14097" max="14097" width="12.34765625" customWidth="1"/>
+    <col min="14339" max="14339" width="56.6484375" customWidth="1"/>
+    <col min="14340" max="14340" width="14.1484375" customWidth="1"/>
+    <col min="14341" max="14341" width="13.1484375" customWidth="1"/>
+    <col min="14342" max="14342" width="12.84765625" customWidth="1"/>
+    <col min="14343" max="14343" width="13.6484375" customWidth="1"/>
     <col min="14344" max="14345" width="13" customWidth="1"/>
-    <col min="14346" max="14346" width="12.6640625" customWidth="1"/>
-    <col min="14347" max="14347" width="11.33203125" customWidth="1"/>
-    <col min="14348" max="14348" width="12.33203125" customWidth="1"/>
+    <col min="14346" max="14346" width="12.6484375" customWidth="1"/>
+    <col min="14347" max="14347" width="11.34765625" customWidth="1"/>
+    <col min="14348" max="14348" width="12.34765625" customWidth="1"/>
     <col min="14349" max="14349" width="13" customWidth="1"/>
-    <col min="14350" max="14350" width="11.83203125" customWidth="1"/>
-    <col min="14351" max="14351" width="12.1640625" customWidth="1"/>
-    <col min="14352" max="14352" width="11.6640625" customWidth="1"/>
-    <col min="14353" max="14353" width="12.33203125" customWidth="1"/>
-    <col min="14595" max="14595" width="56.6640625" customWidth="1"/>
-    <col min="14596" max="14596" width="14.1640625" customWidth="1"/>
-    <col min="14597" max="14597" width="13.1640625" customWidth="1"/>
-    <col min="14598" max="14598" width="12.83203125" customWidth="1"/>
-    <col min="14599" max="14599" width="13.6640625" customWidth="1"/>
+    <col min="14350" max="14350" width="11.84765625" customWidth="1"/>
+    <col min="14351" max="14351" width="12.1484375" customWidth="1"/>
+    <col min="14352" max="14352" width="11.6484375" customWidth="1"/>
+    <col min="14353" max="14353" width="12.34765625" customWidth="1"/>
+    <col min="14595" max="14595" width="56.6484375" customWidth="1"/>
+    <col min="14596" max="14596" width="14.1484375" customWidth="1"/>
+    <col min="14597" max="14597" width="13.1484375" customWidth="1"/>
+    <col min="14598" max="14598" width="12.84765625" customWidth="1"/>
+    <col min="14599" max="14599" width="13.6484375" customWidth="1"/>
     <col min="14600" max="14601" width="13" customWidth="1"/>
-    <col min="14602" max="14602" width="12.6640625" customWidth="1"/>
-    <col min="14603" max="14603" width="11.33203125" customWidth="1"/>
-    <col min="14604" max="14604" width="12.33203125" customWidth="1"/>
+    <col min="14602" max="14602" width="12.6484375" customWidth="1"/>
+    <col min="14603" max="14603" width="11.34765625" customWidth="1"/>
+    <col min="14604" max="14604" width="12.34765625" customWidth="1"/>
     <col min="14605" max="14605" width="13" customWidth="1"/>
-    <col min="14606" max="14606" width="11.83203125" customWidth="1"/>
-    <col min="14607" max="14607" width="12.1640625" customWidth="1"/>
-    <col min="14608" max="14608" width="11.6640625" customWidth="1"/>
-    <col min="14609" max="14609" width="12.33203125" customWidth="1"/>
-    <col min="14851" max="14851" width="56.6640625" customWidth="1"/>
-    <col min="14852" max="14852" width="14.1640625" customWidth="1"/>
-    <col min="14853" max="14853" width="13.1640625" customWidth="1"/>
-    <col min="14854" max="14854" width="12.83203125" customWidth="1"/>
-    <col min="14855" max="14855" width="13.6640625" customWidth="1"/>
+    <col min="14606" max="14606" width="11.84765625" customWidth="1"/>
+    <col min="14607" max="14607" width="12.1484375" customWidth="1"/>
+    <col min="14608" max="14608" width="11.6484375" customWidth="1"/>
+    <col min="14609" max="14609" width="12.34765625" customWidth="1"/>
+    <col min="14851" max="14851" width="56.6484375" customWidth="1"/>
+    <col min="14852" max="14852" width="14.1484375" customWidth="1"/>
+    <col min="14853" max="14853" width="13.1484375" customWidth="1"/>
+    <col min="14854" max="14854" width="12.84765625" customWidth="1"/>
+    <col min="14855" max="14855" width="13.6484375" customWidth="1"/>
     <col min="14856" max="14857" width="13" customWidth="1"/>
-    <col min="14858" max="14858" width="12.6640625" customWidth="1"/>
-    <col min="14859" max="14859" width="11.33203125" customWidth="1"/>
-    <col min="14860" max="14860" width="12.33203125" customWidth="1"/>
+    <col min="14858" max="14858" width="12.6484375" customWidth="1"/>
+    <col min="14859" max="14859" width="11.34765625" customWidth="1"/>
+    <col min="14860" max="14860" width="12.34765625" customWidth="1"/>
     <col min="14861" max="14861" width="13" customWidth="1"/>
-    <col min="14862" max="14862" width="11.83203125" customWidth="1"/>
-    <col min="14863" max="14863" width="12.1640625" customWidth="1"/>
-    <col min="14864" max="14864" width="11.6640625" customWidth="1"/>
-    <col min="14865" max="14865" width="12.33203125" customWidth="1"/>
-    <col min="15107" max="15107" width="56.6640625" customWidth="1"/>
-    <col min="15108" max="15108" width="14.1640625" customWidth="1"/>
-    <col min="15109" max="15109" width="13.1640625" customWidth="1"/>
-    <col min="15110" max="15110" width="12.83203125" customWidth="1"/>
-    <col min="15111" max="15111" width="13.6640625" customWidth="1"/>
+    <col min="14862" max="14862" width="11.84765625" customWidth="1"/>
+    <col min="14863" max="14863" width="12.1484375" customWidth="1"/>
+    <col min="14864" max="14864" width="11.6484375" customWidth="1"/>
+    <col min="14865" max="14865" width="12.34765625" customWidth="1"/>
+    <col min="15107" max="15107" width="56.6484375" customWidth="1"/>
+    <col min="15108" max="15108" width="14.1484375" customWidth="1"/>
+    <col min="15109" max="15109" width="13.1484375" customWidth="1"/>
+    <col min="15110" max="15110" width="12.84765625" customWidth="1"/>
+    <col min="15111" max="15111" width="13.6484375" customWidth="1"/>
     <col min="15112" max="15113" width="13" customWidth="1"/>
-    <col min="15114" max="15114" width="12.6640625" customWidth="1"/>
-    <col min="15115" max="15115" width="11.33203125" customWidth="1"/>
-    <col min="15116" max="15116" width="12.33203125" customWidth="1"/>
+    <col min="15114" max="15114" width="12.6484375" customWidth="1"/>
+    <col min="15115" max="15115" width="11.34765625" customWidth="1"/>
+    <col min="15116" max="15116" width="12.34765625" customWidth="1"/>
     <col min="15117" max="15117" width="13" customWidth="1"/>
-    <col min="15118" max="15118" width="11.83203125" customWidth="1"/>
-    <col min="15119" max="15119" width="12.1640625" customWidth="1"/>
-    <col min="15120" max="15120" width="11.6640625" customWidth="1"/>
-    <col min="15121" max="15121" width="12.33203125" customWidth="1"/>
-    <col min="15363" max="15363" width="56.6640625" customWidth="1"/>
-    <col min="15364" max="15364" width="14.1640625" customWidth="1"/>
-    <col min="15365" max="15365" width="13.1640625" customWidth="1"/>
-    <col min="15366" max="15366" width="12.83203125" customWidth="1"/>
-    <col min="15367" max="15367" width="13.6640625" customWidth="1"/>
+    <col min="15118" max="15118" width="11.84765625" customWidth="1"/>
+    <col min="15119" max="15119" width="12.1484375" customWidth="1"/>
+    <col min="15120" max="15120" width="11.6484375" customWidth="1"/>
+    <col min="15121" max="15121" width="12.34765625" customWidth="1"/>
+    <col min="15363" max="15363" width="56.6484375" customWidth="1"/>
+    <col min="15364" max="15364" width="14.1484375" customWidth="1"/>
+    <col min="15365" max="15365" width="13.1484375" customWidth="1"/>
+    <col min="15366" max="15366" width="12.84765625" customWidth="1"/>
+    <col min="15367" max="15367" width="13.6484375" customWidth="1"/>
     <col min="15368" max="15369" width="13" customWidth="1"/>
-    <col min="15370" max="15370" width="12.6640625" customWidth="1"/>
-    <col min="15371" max="15371" width="11.33203125" customWidth="1"/>
-    <col min="15372" max="15372" width="12.33203125" customWidth="1"/>
+    <col min="15370" max="15370" width="12.6484375" customWidth="1"/>
+    <col min="15371" max="15371" width="11.34765625" customWidth="1"/>
+    <col min="15372" max="15372" width="12.34765625" customWidth="1"/>
     <col min="15373" max="15373" width="13" customWidth="1"/>
-    <col min="15374" max="15374" width="11.83203125" customWidth="1"/>
-    <col min="15375" max="15375" width="12.1640625" customWidth="1"/>
-    <col min="15376" max="15376" width="11.6640625" customWidth="1"/>
-    <col min="15377" max="15377" width="12.33203125" customWidth="1"/>
-    <col min="15619" max="15619" width="56.6640625" customWidth="1"/>
-    <col min="15620" max="15620" width="14.1640625" customWidth="1"/>
-    <col min="15621" max="15621" width="13.1640625" customWidth="1"/>
-    <col min="15622" max="15622" width="12.83203125" customWidth="1"/>
-    <col min="15623" max="15623" width="13.6640625" customWidth="1"/>
+    <col min="15374" max="15374" width="11.84765625" customWidth="1"/>
+    <col min="15375" max="15375" width="12.1484375" customWidth="1"/>
+    <col min="15376" max="15376" width="11.6484375" customWidth="1"/>
+    <col min="15377" max="15377" width="12.34765625" customWidth="1"/>
+    <col min="15619" max="15619" width="56.6484375" customWidth="1"/>
+    <col min="15620" max="15620" width="14.1484375" customWidth="1"/>
+    <col min="15621" max="15621" width="13.1484375" customWidth="1"/>
+    <col min="15622" max="15622" width="12.84765625" customWidth="1"/>
+    <col min="15623" max="15623" width="13.6484375" customWidth="1"/>
     <col min="15624" max="15625" width="13" customWidth="1"/>
-    <col min="15626" max="15626" width="12.6640625" customWidth="1"/>
-    <col min="15627" max="15627" width="11.33203125" customWidth="1"/>
-    <col min="15628" max="15628" width="12.33203125" customWidth="1"/>
+    <col min="15626" max="15626" width="12.6484375" customWidth="1"/>
+    <col min="15627" max="15627" width="11.34765625" customWidth="1"/>
+    <col min="15628" max="15628" width="12.34765625" customWidth="1"/>
     <col min="15629" max="15629" width="13" customWidth="1"/>
-    <col min="15630" max="15630" width="11.83203125" customWidth="1"/>
-    <col min="15631" max="15631" width="12.1640625" customWidth="1"/>
-    <col min="15632" max="15632" width="11.6640625" customWidth="1"/>
-    <col min="15633" max="15633" width="12.33203125" customWidth="1"/>
-    <col min="15875" max="15875" width="56.6640625" customWidth="1"/>
-    <col min="15876" max="15876" width="14.1640625" customWidth="1"/>
-    <col min="15877" max="15877" width="13.1640625" customWidth="1"/>
-    <col min="15878" max="15878" width="12.83203125" customWidth="1"/>
-    <col min="15879" max="15879" width="13.6640625" customWidth="1"/>
+    <col min="15630" max="15630" width="11.84765625" customWidth="1"/>
+    <col min="15631" max="15631" width="12.1484375" customWidth="1"/>
+    <col min="15632" max="15632" width="11.6484375" customWidth="1"/>
+    <col min="15633" max="15633" width="12.34765625" customWidth="1"/>
+    <col min="15875" max="15875" width="56.6484375" customWidth="1"/>
+    <col min="15876" max="15876" width="14.1484375" customWidth="1"/>
+    <col min="15877" max="15877" width="13.1484375" customWidth="1"/>
+    <col min="15878" max="15878" width="12.84765625" customWidth="1"/>
+    <col min="15879" max="15879" width="13.6484375" customWidth="1"/>
     <col min="15880" max="15881" width="13" customWidth="1"/>
-    <col min="15882" max="15882" width="12.6640625" customWidth="1"/>
-    <col min="15883" max="15883" width="11.33203125" customWidth="1"/>
-    <col min="15884" max="15884" width="12.33203125" customWidth="1"/>
+    <col min="15882" max="15882" width="12.6484375" customWidth="1"/>
+    <col min="15883" max="15883" width="11.34765625" customWidth="1"/>
+    <col min="15884" max="15884" width="12.34765625" customWidth="1"/>
     <col min="15885" max="15885" width="13" customWidth="1"/>
-    <col min="15886" max="15886" width="11.83203125" customWidth="1"/>
-    <col min="15887" max="15887" width="12.1640625" customWidth="1"/>
-    <col min="15888" max="15888" width="11.6640625" customWidth="1"/>
-    <col min="15889" max="15889" width="12.33203125" customWidth="1"/>
-    <col min="16131" max="16131" width="56.6640625" customWidth="1"/>
-    <col min="16132" max="16132" width="14.1640625" customWidth="1"/>
-    <col min="16133" max="16133" width="13.1640625" customWidth="1"/>
-    <col min="16134" max="16134" width="12.83203125" customWidth="1"/>
-    <col min="16135" max="16135" width="13.6640625" customWidth="1"/>
+    <col min="15886" max="15886" width="11.84765625" customWidth="1"/>
+    <col min="15887" max="15887" width="12.1484375" customWidth="1"/>
+    <col min="15888" max="15888" width="11.6484375" customWidth="1"/>
+    <col min="15889" max="15889" width="12.34765625" customWidth="1"/>
+    <col min="16131" max="16131" width="56.6484375" customWidth="1"/>
+    <col min="16132" max="16132" width="14.1484375" customWidth="1"/>
+    <col min="16133" max="16133" width="13.1484375" customWidth="1"/>
+    <col min="16134" max="16134" width="12.84765625" customWidth="1"/>
+    <col min="16135" max="16135" width="13.6484375" customWidth="1"/>
     <col min="16136" max="16137" width="13" customWidth="1"/>
-    <col min="16138" max="16138" width="12.6640625" customWidth="1"/>
-    <col min="16139" max="16139" width="11.33203125" customWidth="1"/>
-    <col min="16140" max="16140" width="12.33203125" customWidth="1"/>
+    <col min="16138" max="16138" width="12.6484375" customWidth="1"/>
+    <col min="16139" max="16139" width="11.34765625" customWidth="1"/>
+    <col min="16140" max="16140" width="12.34765625" customWidth="1"/>
     <col min="16141" max="16141" width="13" customWidth="1"/>
-    <col min="16142" max="16142" width="11.83203125" customWidth="1"/>
-    <col min="16143" max="16143" width="12.1640625" customWidth="1"/>
-    <col min="16144" max="16144" width="11.6640625" customWidth="1"/>
-    <col min="16145" max="16145" width="12.33203125" customWidth="1"/>
+    <col min="16142" max="16142" width="11.84765625" customWidth="1"/>
+    <col min="16143" max="16143" width="12.1484375" customWidth="1"/>
+    <col min="16144" max="16144" width="11.6484375" customWidth="1"/>
+    <col min="16145" max="16145" width="12.34765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1780,7 +1783,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -1833,7 +1836,7 @@
         <v>38.799999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1886,7 +1889,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -1939,7 +1942,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -1992,7 +1995,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2045,7 +2048,7 @@
         <v>28.6</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2098,7 +2101,7 @@
         <v>35.299999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2151,7 +2154,7 @@
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2204,7 +2207,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -2257,7 +2260,7 @@
         <v>47.2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -2310,7 +2313,7 @@
         <v>34.700000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -2363,7 +2366,7 @@
         <v>40.799999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2416,7 +2419,7 @@
         <v>36.700000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
@@ -2469,7 +2472,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
@@ -2522,7 +2525,7 @@
         <v>39.5</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A16" s="4" t="s">
         <v>29</v>
       </c>
@@ -2575,7 +2578,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
@@ -2628,7 +2631,7 @@
         <v>27.4</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A18" s="4" t="s">
         <v>31</v>
       </c>
@@ -2681,7 +2684,7 @@
         <v>33.700000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A19" s="4" t="s">
         <v>32</v>
       </c>
@@ -2734,7 +2737,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -2783,7 +2786,7 @@
       </c>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -2832,7 +2835,7 @@
       </c>
       <c r="Q21" s="8"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -2857,7 +2860,9 @@
       <c r="H22" s="7">
         <v>0.11103686999089901</v>
       </c>
-      <c r="I22" s="7"/>
+      <c r="I22" s="7">
+        <v>9.7870760040251206E-2</v>
+      </c>
       <c r="J22" s="8">
         <v>32.700000000000003</v>
       </c>
@@ -2879,9 +2884,11 @@
       <c r="P22" s="8">
         <v>28.7</v>
       </c>
-      <c r="Q22" s="8"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q22" s="19">
+        <v>34.700000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -2906,7 +2913,9 @@
       <c r="H23" s="7">
         <v>-0.27869501119798001</v>
       </c>
-      <c r="I23" s="7"/>
+      <c r="I23" s="7">
+        <v>0.16271572368472501</v>
+      </c>
       <c r="J23" s="8">
         <v>37.200000000000003</v>
       </c>
@@ -2928,9 +2937,11 @@
       <c r="P23" s="8">
         <v>27</v>
       </c>
-      <c r="Q23" s="8"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q23" s="8">
+        <v>45.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -2983,7 +2994,7 @@
         <v>43.2</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -3036,7 +3047,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -3089,7 +3100,7 @@
         <v>41.2</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A27" s="4" t="s">
         <v>40</v>
       </c>
@@ -3138,7 +3149,7 @@
       </c>
       <c r="Q27" s="6"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A28" s="4" t="s">
         <v>41</v>
       </c>
@@ -3187,7 +3198,7 @@
       </c>
       <c r="Q28" s="6"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A29" s="4" t="s">
         <v>42</v>
       </c>
@@ -3236,7 +3247,7 @@
       </c>
       <c r="Q29" s="6"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A30" s="4" t="s">
         <v>43</v>
       </c>
@@ -3285,7 +3296,7 @@
       </c>
       <c r="Q30" s="6"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A31" s="4" t="s">
         <v>44</v>
       </c>
@@ -3334,7 +3345,7 @@
       </c>
       <c r="Q31" s="6"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A32" s="4" t="s">
         <v>45</v>
       </c>
@@ -3383,7 +3394,7 @@
       </c>
       <c r="Q32" s="6"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A33" s="4" t="s">
         <v>46</v>
       </c>
@@ -3432,7 +3443,7 @@
       </c>
       <c r="Q33" s="6"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -3481,7 +3492,7 @@
       </c>
       <c r="Q34" s="8"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -3530,7 +3541,7 @@
       </c>
       <c r="Q35" s="8"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -3579,7 +3590,7 @@
       </c>
       <c r="Q36" s="8"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -3628,7 +3639,7 @@
       </c>
       <c r="Q37" s="8"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -3677,7 +3688,7 @@
       </c>
       <c r="Q38" s="8"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -3726,7 +3737,7 @@
       </c>
       <c r="Q39" s="8"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -3775,7 +3786,7 @@
       </c>
       <c r="Q40" s="8"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -3824,7 +3835,7 @@
       </c>
       <c r="Q41" s="8"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A42" s="4" t="s">
         <v>55</v>
       </c>
@@ -3873,7 +3884,7 @@
       </c>
       <c r="Q42" s="6"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A43" s="4" t="s">
         <v>56</v>
       </c>
@@ -3922,7 +3933,7 @@
       </c>
       <c r="Q43" s="6"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A44" s="4" t="s">
         <v>57</v>
       </c>
@@ -3971,7 +3982,7 @@
       </c>
       <c r="Q44" s="6"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A45" s="4" t="s">
         <v>58</v>
       </c>
@@ -4020,7 +4031,7 @@
       </c>
       <c r="Q45" s="6"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A46" s="4" t="s">
         <v>59</v>
       </c>
@@ -4069,7 +4080,7 @@
       </c>
       <c r="Q46" s="6"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A47" s="4" t="s">
         <v>60</v>
       </c>
@@ -4118,7 +4129,7 @@
       </c>
       <c r="Q47" s="6"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A48" s="4" t="s">
         <v>61</v>
       </c>
@@ -4167,7 +4178,7 @@
       </c>
       <c r="Q48" s="6"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A49" t="s">
         <v>62</v>
       </c>
@@ -4216,7 +4227,7 @@
       </c>
       <c r="Q49" s="8"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -4265,7 +4276,7 @@
       </c>
       <c r="Q50" s="8"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -4314,7 +4325,7 @@
       </c>
       <c r="Q51" s="8"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A52" t="s">
         <v>65</v>
       </c>
@@ -4363,7 +4374,7 @@
       </c>
       <c r="Q52" s="8"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -4412,7 +4423,7 @@
       </c>
       <c r="Q53" s="8"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A54" t="s">
         <v>67</v>
       </c>
@@ -4461,7 +4472,7 @@
       </c>
       <c r="Q54" s="8"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A55" t="s">
         <v>68</v>
       </c>
@@ -4510,7 +4521,7 @@
       </c>
       <c r="Q55" s="8"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A56" t="s">
         <v>69</v>
       </c>
@@ -4559,7 +4570,7 @@
       </c>
       <c r="Q56" s="8"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A57" s="4" t="s">
         <v>70</v>
       </c>
@@ -4608,7 +4619,7 @@
       </c>
       <c r="Q57" s="6"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A58" s="4" t="s">
         <v>71</v>
       </c>
@@ -4657,7 +4668,7 @@
       </c>
       <c r="Q58" s="6"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A59" s="4" t="s">
         <v>72</v>
       </c>
@@ -4706,7 +4717,7 @@
       </c>
       <c r="Q59" s="6"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A60" s="4" t="s">
         <v>73</v>
       </c>
@@ -4755,7 +4766,7 @@
       </c>
       <c r="Q60" s="6"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A61" s="4" t="s">
         <v>74</v>
       </c>
@@ -4804,7 +4815,7 @@
       </c>
       <c r="Q61" s="6"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A62" s="4" t="s">
         <v>75</v>
       </c>
@@ -4853,7 +4864,7 @@
       </c>
       <c r="Q62" s="6"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A63" s="4" t="s">
         <v>76</v>
       </c>
@@ -4902,7 +4913,7 @@
       </c>
       <c r="Q63" s="6"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A64" s="4" t="s">
         <v>77</v>
       </c>
@@ -4951,7 +4962,7 @@
       </c>
       <c r="Q64" s="6"/>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A65" s="4" t="s">
         <v>78</v>
       </c>
@@ -5000,7 +5011,7 @@
       </c>
       <c r="Q65" s="6"/>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A66" t="s">
         <v>79</v>
       </c>
@@ -5049,7 +5060,7 @@
       </c>
       <c r="Q66" s="8"/>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A67" t="s">
         <v>80</v>
       </c>
@@ -5098,7 +5109,7 @@
       </c>
       <c r="Q67" s="8"/>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A68" t="s">
         <v>81</v>
       </c>
@@ -5147,7 +5158,7 @@
       </c>
       <c r="Q68" s="8"/>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A69" t="s">
         <v>82</v>
       </c>
@@ -5196,7 +5207,7 @@
       </c>
       <c r="Q69" s="8"/>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A70" t="s">
         <v>83</v>
       </c>
@@ -5245,7 +5256,7 @@
       </c>
       <c r="Q70" s="8"/>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A71" s="9" t="s">
         <v>84</v>
       </c>
@@ -5279,7 +5290,7 @@
       </c>
       <c r="I71" s="10">
         <f t="shared" si="0"/>
-        <v>0.1773078509594837</v>
+        <v>0.17321962408148406</v>
       </c>
       <c r="J71" s="11">
         <f t="shared" si="0"/>
@@ -5311,10 +5322,10 @@
       </c>
       <c r="Q71" s="11">
         <f t="shared" si="0"/>
-        <v>35.433333333333337</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+        <v>35.821739130434786</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A72" s="1" t="s">
         <v>0</v>
       </c>
@@ -5367,7 +5378,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.6">
       <c r="B76" s="12" t="s">
         <v>85</v>
       </c>
@@ -5378,7 +5389,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.6">
       <c r="B77" s="14" t="s">
         <v>88</v>
       </c>
@@ -5391,7 +5402,7 @@
         <v>39.433333333333351</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.6">
       <c r="B78" s="14" t="s">
         <v>89</v>
       </c>
@@ -5404,7 +5415,7 @@
         <v>34.676811594202896</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.6">
       <c r="B79" s="14" t="s">
         <v>90</v>
       </c>
@@ -5417,7 +5428,7 @@
         <v>32.372463768115949</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.6">
       <c r="B80" s="14" t="s">
         <v>91</v>
       </c>
@@ -5430,7 +5441,7 @@
         <v>31.473913043478266</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.6">
       <c r="B81" s="17" t="s">
         <v>92</v>
       </c>
@@ -5443,7 +5454,7 @@
         <v>31.089855072463774</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.6">
       <c r="B82" s="17" t="s">
         <v>93</v>
       </c>
@@ -5456,7 +5467,7 @@
         <v>31.704347826086948</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.6">
       <c r="B83" s="17" t="s">
         <v>94</v>
       </c>
@@ -5469,34 +5480,34 @@
         <v>31.153623188405788</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.6">
       <c r="B84" s="17" t="s">
         <v>108</v>
       </c>
       <c r="C84" s="15">
         <f>I71</f>
-        <v>0.1773078509594837</v>
+        <v>0.17321962408148406</v>
       </c>
       <c r="D84" s="16">
         <f>Q71</f>
-        <v>35.433333333333337</v>
-      </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+        <v>35.821739130434786</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.6">
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
       <c r="D85" s="8"/>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.6">
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
       <c r="D86" s="8"/>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.6">
       <c r="B87" s="7"/>
       <c r="D87" s="18"/>
     </row>
-    <row r="88" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A88" s="1" t="s">
         <v>95</v>
       </c>
@@ -5549,7 +5560,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A89" t="s">
         <v>96</v>
       </c>
@@ -5618,7 +5629,7 @@
         <v>29.824999999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A90" t="s">
         <v>97</v>
       </c>
@@ -5687,7 +5698,7 @@
         <v>36.75</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A91" t="s">
         <v>98</v>
       </c>
@@ -5756,7 +5767,7 @@
         <v>34.5</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A92" t="s">
         <v>99</v>
       </c>
@@ -5790,7 +5801,7 @@
       </c>
       <c r="I92" s="5">
         <f t="shared" ref="I92" si="10">AVERAGE(I20:I26)</f>
-        <v>0.30660497129034686</v>
+        <v>0.23608027951920335</v>
       </c>
       <c r="J92" s="8">
         <f t="shared" si="9"/>
@@ -5822,10 +5833,10 @@
       </c>
       <c r="Q92" s="6">
         <f t="shared" ref="Q92" si="11">AVERAGE(Q20:Q26)</f>
-        <v>41.266666666666666</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+        <v>40.720000000000006</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A93" t="s">
         <v>100</v>
       </c>
@@ -5894,7 +5905,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A94" t="s">
         <v>101</v>
       </c>
@@ -5963,7 +5974,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A95" t="s">
         <v>102</v>
       </c>
@@ -6032,7 +6043,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A96" t="s">
         <v>103</v>
       </c>
@@ -6101,7 +6112,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A97" t="s">
         <v>104</v>
       </c>
@@ -6170,7 +6181,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A98" t="s">
         <v>105</v>
       </c>
@@ -6239,7 +6250,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="99" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:17" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A99" s="1" t="s">
         <v>95</v>
       </c>
@@ -6311,7 +6322,7 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added results for 4a and 4b
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fairouz\Desktop\cognitive project\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0FA808-9912-46FA-9F24-04856CCB2281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A66004-C0EA-47A0-8FBF-4571A9FB43B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{EFD26FD0-07EC-0644-AECA-4418AC46A54A}"/>
   </bookViews>
@@ -402,7 +402,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,6 +445,12 @@
         <bgColor indexed="27"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -459,7 +465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -505,7 +511,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -825,9 +834,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A8C6A9-729D-1346-9EE7-9CB9A898ACBA}">
   <dimension ref="A1:Q99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -2762,7 +2771,9 @@
       <c r="H20" s="7">
         <v>0.20716875720084402</v>
       </c>
-      <c r="I20" s="7"/>
+      <c r="I20" s="7">
+        <v>0.17092160392123801</v>
+      </c>
       <c r="J20" s="8">
         <v>27.3</v>
       </c>
@@ -2784,7 +2795,9 @@
       <c r="P20" s="8">
         <v>39.4</v>
       </c>
-      <c r="Q20" s="8"/>
+      <c r="Q20" s="8">
+        <v>40.299999999999997</v>
+      </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A21" t="s">
@@ -2811,7 +2824,9 @@
       <c r="H21" s="7">
         <v>0.53144059015965206</v>
       </c>
-      <c r="I21" s="7"/>
+      <c r="I21" s="7">
+        <v>-0.16590826535158801</v>
+      </c>
       <c r="J21" s="8">
         <v>23.9</v>
       </c>
@@ -2833,7 +2848,9 @@
       <c r="P21" s="8">
         <v>50.6</v>
       </c>
-      <c r="Q21" s="8"/>
+      <c r="Q21" s="20">
+        <v>26.7</v>
+      </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.6">
       <c r="A22" t="s">
@@ -5290,7 +5307,7 @@
       </c>
       <c r="I71" s="10">
         <f t="shared" si="0"/>
-        <v>0.17321962408148406</v>
+        <v>0.15956258769775133</v>
       </c>
       <c r="J71" s="11">
         <f t="shared" si="0"/>
@@ -5322,7 +5339,7 @@
       </c>
       <c r="Q71" s="11">
         <f t="shared" si="0"/>
-        <v>35.821739130434786</v>
+        <v>35.636000000000003</v>
       </c>
     </row>
     <row r="72" spans="1:17" ht="31.2" x14ac:dyDescent="0.6">
@@ -5486,11 +5503,11 @@
       </c>
       <c r="C84" s="15">
         <f>I71</f>
-        <v>0.17321962408148406</v>
+        <v>0.15956258769775133</v>
       </c>
       <c r="D84" s="16">
         <f>Q71</f>
-        <v>35.821739130434786</v>
+        <v>35.636000000000003</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.6">
@@ -5801,7 +5818,7 @@
       </c>
       <c r="I92" s="5">
         <f t="shared" ref="I92" si="10">AVERAGE(I20:I26)</f>
-        <v>0.23608027951920335</v>
+        <v>0.16934496230938098</v>
       </c>
       <c r="J92" s="8">
         <f t="shared" si="9"/>
@@ -5833,7 +5850,7 @@
       </c>
       <c r="Q92" s="6">
         <f t="shared" ref="Q92" si="11">AVERAGE(Q20:Q26)</f>
-        <v>40.720000000000006</v>
+        <v>38.657142857142858</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.6">

</xml_diff>